<commit_message>
added a 3rd CRM test
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +406,132 @@
         <v>169</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43173</v>
+      </c>
+      <c r="B3">
+        <v>2217.5163287970099</v>
+      </c>
+      <c r="C3">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">100*(B3-C3)/C3</f>
+        <v>0.47513304291331421</v>
+      </c>
+      <c r="E3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43173</v>
+      </c>
+      <c r="B4">
+        <v>2219.6900936089201</v>
+      </c>
+      <c r="C4">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.57362580521877138</v>
+      </c>
+      <c r="E4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43173</v>
+      </c>
+      <c r="B5">
+        <v>2225.21466328611</v>
+      </c>
+      <c r="C5">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.82394273236475046</v>
+      </c>
+      <c r="E5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43173</v>
+      </c>
+      <c r="B6">
+        <v>2221.4246394258698</v>
+      </c>
+      <c r="C6">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.65221766019807736</v>
+      </c>
+      <c r="E6">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43173</v>
+      </c>
+      <c r="B7">
+        <v>2227.6089961644998</v>
+      </c>
+      <c r="C7">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.93242938086476324</v>
+      </c>
+      <c r="E7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E8">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E9">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E10">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first run of the Bermuda Data
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -360,7 +360,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,12 +497,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43185</v>
+      </c>
+      <c r="B8">
+        <v>2216.86593863592</v>
+      </c>
       <c r="C8">
         <v>2207.0300000000002</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.44566402069386341</v>
       </c>
       <c r="E8">
         <v>169</v>

</xml_diff>

<commit_message>
ran the 26 deg samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D16" si="0">100*(B3-C3)/C3</f>
+        <f t="shared" ref="D3:D26" si="0">100*(B3-C3)/C3</f>
         <v>0.47513304291331421</v>
       </c>
       <c r="E3">
@@ -689,6 +689,138 @@
       </c>
       <c r="G16" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43194</v>
+      </c>
+      <c r="B17">
+        <v>2222.7716464551399</v>
+      </c>
+      <c r="C17">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.71325022564893736</v>
+      </c>
+      <c r="E17">
+        <v>169</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E18">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E19">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E20">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E21">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E22">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E23">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E24">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E26">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Titrated 32C @ 4/18/2018
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -369,7 +369,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,27 +740,45 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43208</v>
+      </c>
+      <c r="B19">
+        <v>2224.6526515354399</v>
+      </c>
       <c r="C19">
         <v>2207.0300000000002</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.79847811472611019</v>
       </c>
       <c r="E19">
         <v>169</v>
       </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43208</v>
+      </c>
+      <c r="B20">
+        <v>2223.9979788785199</v>
+      </c>
       <c r="C20">
         <v>2207.0300000000002</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.76881505364764935</v>
       </c>
       <c r="E20">
         <v>169</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Partial Titrate @ 36C
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -369,7 +369,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,18 +824,28 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43215</v>
+      </c>
+      <c r="B23">
+        <v>2218.2645308156002</v>
+      </c>
       <c r="C23">
         <v>2207.0300000000002</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.50903389693841994</v>
       </c>
       <c r="E23">
         <v>169</v>
       </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
       <c r="C24">
         <v>2207.0300000000002</v>
       </c>

</xml_diff>

<commit_message>
Titrated 24-36 @ 5/9/18
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -368,8 +368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,15 +869,27 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43229</v>
+      </c>
+      <c r="B25">
+        <v>2217.6104390258802</v>
+      </c>
       <c r="C25">
         <v>2207.0300000000002</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.47939715481348089</v>
       </c>
       <c r="E25">
         <v>169</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Titrated 27-34 C @ 5/23/2018
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="E26" sqref="E26:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D26" si="0">100*(B3-C3)/C3</f>
+        <f t="shared" ref="D3:D34" si="0">100*(B3-C3)/C3</f>
         <v>0.47513304291331421</v>
       </c>
       <c r="E3">
@@ -893,14 +893,122 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B26">
+        <v>2214.1672841453801</v>
+      </c>
       <c r="C26">
         <v>2207.0300000000002</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
+        <v>0.32338863293112952</v>
+      </c>
+      <c r="E26">
+        <v>169</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
         <v>-100</v>
       </c>
-      <c r="E26">
+      <c r="E27">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E28">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E29">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E30">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E31">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E32">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E33">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="E34">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pushing first 11 samples with replicates from 20190112 20 degrees light samples Moorea
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Without Junk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRM bottle already opened </t>
+  </si>
+  <si>
+    <t>New CRM bottle</t>
   </si>
 </sst>
 </file>
@@ -368,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:E34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,6 +384,8 @@
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -917,27 +925,45 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43503</v>
+      </c>
+      <c r="B27">
+        <v>2189.90222552467</v>
+      </c>
       <c r="C27">
         <v>2207.0300000000002</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>-0.77605535381622215</v>
       </c>
       <c r="E27">
         <v>169</v>
       </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43503</v>
+      </c>
+      <c r="B28">
+        <v>2204.7327702513298</v>
+      </c>
       <c r="C28">
         <v>2207.0300000000002</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>-0.10408692898013895</v>
       </c>
       <c r="E28">
         <v>169</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commiting the TA, mass and overall data to Titrator repo from 02082019, includes redos of PA6 and PA11 from 20 degrees, a junk sample, and 11 samples from 24 degrees collected on January 12 2019 in Moorea
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -375,7 +375,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,15 +967,24 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43504</v>
+      </c>
+      <c r="B29">
+        <v>2206.2235349408302</v>
+      </c>
       <c r="C29">
         <v>2207.0300000000002</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>-3.6540738420865269E-2</v>
       </c>
       <c r="E29">
         <v>169</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
uploading and commiting the TA data for temperatures 30, 31, 32, and 35 from 01/12 for the light treatment in Moorea, included CRM in betwee 22 samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -53,7 +53,10 @@
     <t xml:space="preserve">CRM bottle already opened </t>
   </si>
   <si>
-    <t>New CRM bottle</t>
+    <t>New CRM bottle (opened 02/07)</t>
+  </si>
+  <si>
+    <t>New CRM bottle (opened 02/14)</t>
   </si>
 </sst>
 </file>
@@ -374,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,7 +387,7 @@
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -988,18 +991,28 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43510</v>
+      </c>
+      <c r="B30">
+        <v>2219.88</v>
+      </c>
       <c r="C30">
         <v>2207.0300000000002</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.58223041825439203</v>
       </c>
       <c r="E30">
         <v>169</v>
       </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
       <c r="C31">
         <v>2207.0300000000002</v>
       </c>

</xml_diff>

<commit_message>
TA values calculated for temperture 38 degrees from jan 12 and temperature 20 degrees from jan 15th in Moorea
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -377,8 +377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,16 +1012,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1">
+        <v>43511</v>
+      </c>
+      <c r="B31">
+        <v>2210.7950000000001</v>
+      </c>
       <c r="C31">
         <v>2207.0300000000002</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.17059124706052353</v>
       </c>
       <c r="E31">
         <v>169</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
committed the data processed on 02182019 for light calcification TA values for samples taken on jan 15 in moorea at temperatures 24, 28, 30, 31
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -378,7 +378,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,15 +1033,24 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43514</v>
+      </c>
+      <c r="B32">
+        <v>2216.788</v>
+      </c>
       <c r="C32">
         <v>2207.0300000000002</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.44213263979192896</v>
       </c>
       <c r="E32">
         <v>169</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commiting the TA values calculated on 02192019 for bottles with temperatures 32, 35 and 39 collected in January in moorea on 0115, last set of temperatures and TA measurements
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>New CRM bottle (opened 02/14)</t>
+  </si>
+  <si>
+    <t>2/19/12019</t>
+  </si>
+  <si>
+    <t>New CRM bottle (opened 02/19)</t>
   </si>
 </sst>
 </file>
@@ -92,9 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
@@ -1053,27 +1062,96 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <v>2226.3739999999998</v>
+      </c>
       <c r="C33">
         <v>2207.0300000000002</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
+        <v>0.87647200083368126</v>
+      </c>
+      <c r="E33">
+        <v>169</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
         <v>-100</v>
       </c>
-      <c r="E33">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <v>2207.0300000000002</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
+      <c r="E34">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D39" si="1">100*(B35-C35)/C35</f>
         <v>-100</v>
       </c>
-      <c r="E34">
+      <c r="E35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="E36">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="E37">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="E38">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="E39">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding all Oregon samples Ocean-Tide Pool4
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>New CRM bottle (opened 02/19)</t>
+  </si>
+  <si>
+    <t>Opened CRM (08/08/2019)</t>
+  </si>
+  <si>
+    <t>Opened CRM (08/30/2019)</t>
+  </si>
+  <si>
+    <t>Opened CRM (8/30/2019)</t>
   </si>
 </sst>
 </file>
@@ -384,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,75 +1093,171 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43705</v>
+      </c>
+      <c r="B34">
+        <v>2215.4690000000001</v>
+      </c>
       <c r="C34">
         <v>2207.0300000000002</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>0.38236906612052624</v>
       </c>
       <c r="E34">
         <v>169</v>
       </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43705</v>
+      </c>
+      <c r="B35">
+        <v>2207.4969999999998</v>
+      </c>
       <c r="C35">
         <v>2207.0300000000002</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D39" si="1">100*(B35-C35)/C35</f>
-        <v>-100</v>
+        <f t="shared" ref="D35:D41" si="1">100*(B35-C35)/C35</f>
+        <v>2.115965800191404E-2</v>
       </c>
       <c r="E35">
         <v>169</v>
       </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43705</v>
+      </c>
+      <c r="B36">
+        <v>2207.2800000000002</v>
+      </c>
       <c r="C36">
         <v>2207.0300000000002</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
-        <v>-100</v>
+        <v>1.1327440043859847E-2</v>
       </c>
       <c r="E36">
         <v>169</v>
       </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43707</v>
+      </c>
+      <c r="B37">
+        <v>2211.4369999999999</v>
+      </c>
       <c r="C37">
         <v>2207.0300000000002</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
-        <v>-100</v>
+        <v>0.1996801130931477</v>
       </c>
       <c r="E37">
         <v>169</v>
       </c>
+      <c r="F37" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43707</v>
+      </c>
+      <c r="B38">
+        <v>2212.1660000000002</v>
+      </c>
       <c r="C38">
         <v>2207.0300000000002</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
-        <v>-100</v>
+        <v>0.23271092826105522</v>
       </c>
       <c r="E38">
         <v>169</v>
       </c>
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43708</v>
+      </c>
+      <c r="B39">
+        <v>2208.1019999999999</v>
+      </c>
       <c r="C39">
         <v>2207.0300000000002</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
-        <v>-100</v>
+        <v>4.8572062908055692E-2</v>
       </c>
       <c r="E39">
         <v>169</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43709</v>
+      </c>
+      <c r="B40">
+        <v>2215.7841985129398</v>
+      </c>
+      <c r="C40">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>0.39665063514948312</v>
+      </c>
+      <c r="E40">
+        <v>169</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43710</v>
+      </c>
+      <c r="B41">
+        <v>2215.1630609276599</v>
+      </c>
+      <c r="C41">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>0.36850704012449753</v>
+      </c>
+      <c r="E41">
+        <v>169</v>
+      </c>
+      <c r="F41" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Tp 5 and 6
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1124,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D41" si="1">100*(B35-C35)/C35</f>
+        <f t="shared" ref="D35:D42" si="1">100*(B35-C35)/C35</f>
         <v>2.115965800191404E-2</v>
       </c>
       <c r="E35">
@@ -1257,6 +1257,27 @@
         <v>169</v>
       </c>
       <c r="F41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43712</v>
+      </c>
+      <c r="B42">
+        <v>2218.9034025771698</v>
+      </c>
+      <c r="C42">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>0.53798102323799857</v>
+      </c>
+      <c r="E42">
+        <v>169</v>
+      </c>
+      <c r="F42" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding tp 7 and 8 from OR tide pools
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1124,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D42" si="1">100*(B35-C35)/C35</f>
+        <f t="shared" ref="D35:D43" si="1">100*(B35-C35)/C35</f>
         <v>2.115965800191404E-2</v>
       </c>
       <c r="E35">
@@ -1278,6 +1278,27 @@
         <v>169</v>
       </c>
       <c r="F42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43713</v>
+      </c>
+      <c r="B43">
+        <v>2219.0529999999999</v>
+      </c>
+      <c r="C43">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>0.54475924658929342</v>
+      </c>
+      <c r="E43">
+        <v>169</v>
+      </c>
+      <c r="F43" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding TP 9 and 10 to Oregon tide pools TA
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:F43"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1124,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D43" si="1">100*(B35-C35)/C35</f>
+        <f t="shared" ref="D35:D44" si="1">100*(B35-C35)/C35</f>
         <v>2.115965800191404E-2</v>
       </c>
       <c r="E35">
@@ -1299,6 +1299,27 @@
         <v>169</v>
       </c>
       <c r="F43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43715</v>
+      </c>
+      <c r="B44">
+        <v>2212.9281273883298</v>
+      </c>
+      <c r="C44">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>0.26724273744940541</v>
+      </c>
+      <c r="E44">
+        <v>169</v>
+      </c>
+      <c r="F44" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding tp 11 and 12
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Opened CRM (8/30/2019)</t>
+  </si>
+  <si>
+    <t>Opened CRM (9/8/2019)</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1127,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D44" si="1">100*(B35-C35)/C35</f>
+        <f t="shared" ref="D35:D45" si="1">100*(B35-C35)/C35</f>
         <v>2.115965800191404E-2</v>
       </c>
       <c r="E35">
@@ -1321,6 +1324,48 @@
       </c>
       <c r="F44" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43716</v>
+      </c>
+      <c r="B45">
+        <v>2256.8387198168102</v>
+      </c>
+      <c r="C45">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D45">
+        <f>100*(B45-C45)/C45</f>
+        <v>2.2568211495453174</v>
+      </c>
+      <c r="E45">
+        <v>169</v>
+      </c>
+      <c r="F45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43716</v>
+      </c>
+      <c r="B46">
+        <v>2221.5640712207201</v>
+      </c>
+      <c r="C46">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D46">
+        <f>100*(B46-C46)/C46</f>
+        <v>0.65853528138357209</v>
+      </c>
+      <c r="E46">
+        <v>169</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit data files for Hawaii samples run on 20190909 by dani b
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Opened CRM (9/8/2019)</t>
+  </si>
+  <si>
+    <t>Opened CRM (9/8/2019), Dani B</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1130,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D45" si="1">100*(B35-C35)/C35</f>
+        <f t="shared" ref="D35:D44" si="1">100*(B35-C35)/C35</f>
         <v>2.115965800191404E-2</v>
       </c>
       <c r="E35">
@@ -1366,6 +1369,72 @@
       </c>
       <c r="F46" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43717</v>
+      </c>
+      <c r="B47">
+        <v>2214.8376635135801</v>
+      </c>
+      <c r="C47">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ref="D47:D52" si="2">100*(B47-C47)/C47</f>
+        <v>0.35376336133083292</v>
+      </c>
+      <c r="E47">
+        <v>169</v>
+      </c>
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>-100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit hawaii samples, 30 from 20190910, rechecking CRM and last sample
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -402,7 +402,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,12 +1393,24 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43718</v>
+      </c>
+      <c r="B48">
+        <v>2218.7914332390801</v>
+      </c>
       <c r="C48">
         <v>2207.0300000000002</v>
       </c>
       <c r="D48">
         <f t="shared" si="2"/>
-        <v>-100</v>
+        <v>0.53290771938215187</v>
+      </c>
+      <c r="E48">
+        <v>169</v>
+      </c>
+      <c r="F48" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding pH calibration from 10/2/2019 JFields run
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Opened CRM (9/8/2019), Dani B</t>
+  </si>
+  <si>
+    <t>run at beginning of day with new probe</t>
+  </si>
+  <si>
+    <t>run at beginning of day</t>
+  </si>
+  <si>
+    <t>opened crm (9/8/2019); ph calibration off?</t>
+  </si>
+  <si>
+    <t>opened crm (8/7/2019)</t>
   </si>
 </sst>
 </file>
@@ -401,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,40 +1425,79 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43719</v>
+      </c>
+      <c r="B49">
+        <v>2217.19</v>
+      </c>
       <c r="C49">
         <v>2207.0300000000002</v>
       </c>
       <c r="D49">
         <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+        <v>0.46034716338245757</v>
+      </c>
+      <c r="E49">
+        <v>169</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43720</v>
+      </c>
+      <c r="B50">
+        <v>2218.23</v>
+      </c>
       <c r="C50">
         <v>2207.0300000000002</v>
       </c>
       <c r="D50">
         <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+        <v>0.5074693139649129</v>
+      </c>
+      <c r="E50">
+        <v>169</v>
+      </c>
+      <c r="F50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43723</v>
+      </c>
+      <c r="B51">
+        <v>2091.32236590917</v>
+      </c>
       <c r="C51">
         <v>2207.0300000000002</v>
       </c>
       <c r="D51">
         <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+        <v>-5.2426851511230108</v>
+      </c>
+      <c r="E51">
+        <v>169</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>2207.0300000000002</v>
       </c>
       <c r="D52">
         <f t="shared" si="2"/>
         <v>-100</v>
+      </c>
+      <c r="F52" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding crm test from 10.04.2019
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,14 +1489,44 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43742</v>
+      </c>
+      <c r="B52">
+        <v>2275.4950372970102</v>
+      </c>
       <c r="C52">
         <v>2207.0300000000002</v>
       </c>
       <c r="D52">
-        <f t="shared" si="2"/>
-        <v>-100</v>
+        <f>100*(B52-C52)/C52</f>
+        <v>3.1021344203300352</v>
+      </c>
+      <c r="E52">
+        <v>169</v>
       </c>
       <c r="F52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43742</v>
+      </c>
+      <c r="B53">
+        <v>2268.8014966576202</v>
+      </c>
+      <c r="C53">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D53">
+        <f>100*(B53-C53)/C53</f>
+        <v>2.7988516992347177</v>
+      </c>
+      <c r="E53">
+        <v>169</v>
+      </c>
+      <c r="F53" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding crm test from 10.5.2019 for backcalcuation
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>opened crm (8/7/2019)</t>
+  </si>
+  <si>
+    <t>opend crm (10/5/2019</t>
+  </si>
+  <si>
+    <t>opened crm (10/5/2019</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,7 +1400,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D47">
-        <f t="shared" ref="D47:D52" si="2">100*(B47-C47)/C47</f>
+        <f t="shared" ref="D47:D51" si="2">100*(B47-C47)/C47</f>
         <v>0.35376336133083292</v>
       </c>
       <c r="E47">
@@ -1528,6 +1534,48 @@
       </c>
       <c r="F53" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43743</v>
+      </c>
+      <c r="B54">
+        <v>2286.5546243738299</v>
+      </c>
+      <c r="C54">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ref="D54:D55" si="3">100*(B54-C54)/C54</f>
+        <v>3.603241658420127</v>
+      </c>
+      <c r="E54">
+        <v>169</v>
+      </c>
+      <c r="F54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43743</v>
+      </c>
+      <c r="B55">
+        <v>2281.5549225887498</v>
+      </c>
+      <c r="C55">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>3.3767063695894315</v>
+      </c>
+      <c r="E55">
+        <v>169</v>
+      </c>
+      <c r="F55" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
10 samples from Hawaii 10.6.2019
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>opened crm (10/5/2019</t>
+  </si>
+  <si>
+    <t>Raw TA;opened crm (10/5/2019</t>
+  </si>
+  <si>
+    <t>TA Evap;opened crm (10/5/2019</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1553,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D55" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D57" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1576,6 +1582,48 @@
       </c>
       <c r="F55" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43744</v>
+      </c>
+      <c r="B56">
+        <v>2217.7131926780899</v>
+      </c>
+      <c r="C56">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="3"/>
+        <v>0.48405289815225228</v>
+      </c>
+      <c r="E56">
+        <v>169</v>
+      </c>
+      <c r="F56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43744</v>
+      </c>
+      <c r="B57">
+        <v>2210.1355849582301</v>
+      </c>
+      <c r="C57">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="3"/>
+        <v>0.14071330966184797</v>
+      </c>
+      <c r="E57">
+        <v>169</v>
+      </c>
+      <c r="F57" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding test run but issues with CRM so did not run samples today
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>TA Evap;opened crm (10/5/2019</t>
+  </si>
+  <si>
+    <t>opened crm…new crm needed</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1556,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D57" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D58" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1624,6 +1627,27 @@
       </c>
       <c r="F57" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43747</v>
+      </c>
+      <c r="B58">
+        <v>2247.4119999999998</v>
+      </c>
+      <c r="C58">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="3"/>
+        <v>1.8296987354045755</v>
+      </c>
+      <c r="E58">
+        <v>169</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting CRM runs from 10.10.19
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>opened crm…new crm needed</t>
+  </si>
+  <si>
+    <t>Raw TA opened crm 10/10/19</t>
+  </si>
+  <si>
+    <t>TA evap; opened crm 10/10/19</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1562,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D58" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D60" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1648,6 +1654,48 @@
       </c>
       <c r="F58" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43748</v>
+      </c>
+      <c r="B59">
+        <v>2365.5419999999999</v>
+      </c>
+      <c r="C59">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="3"/>
+        <v>7.1821407049292354</v>
+      </c>
+      <c r="E59">
+        <v>169</v>
+      </c>
+      <c r="F59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43748</v>
+      </c>
+      <c r="B60">
+        <v>2357.4589999999998</v>
+      </c>
+      <c r="C60">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="3"/>
+        <v>6.8159019134311549</v>
+      </c>
+      <c r="E60">
+        <v>169</v>
+      </c>
+      <c r="F60" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
10/16/2019 CRM value off - titrator read "Status Not Ok"
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>TA evap; opened crm 10/10/19</t>
+  </si>
+  <si>
+    <t>junk 5 of 6 "Not Ok".  Junk 6 and CRM both inconsistent</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,7 +1565,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D60" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D61" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1696,6 +1699,27 @@
       </c>
       <c r="F60" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43754</v>
+      </c>
+      <c r="B61">
+        <v>3167.9356699999998</v>
+      </c>
+      <c r="C61">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="3"/>
+        <v>43.53840545891989</v>
+      </c>
+      <c r="E61">
+        <v>169</v>
+      </c>
+      <c r="F61" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Titration with new acid dosing hose, new CRM, new pH buffers 11/8/2019
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>junk 5 of 6 "Not Ok".  Junk 6 and CRM both inconsistent</t>
+  </si>
+  <si>
+    <t>new crm, fresh pH cal solutions, new hose for acid dosing</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1568,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D61" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D62" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1720,6 +1723,27 @@
       </c>
       <c r="F61" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43777</v>
+      </c>
+      <c r="B62">
+        <v>2142.32205763918</v>
+      </c>
+      <c r="C62">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="3"/>
+        <v>-2.9319013498149182</v>
+      </c>
+      <c r="E62">
+        <v>169</v>
+      </c>
+      <c r="F62" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested CRM accuracy with new dosing hose, and with crm and pH buffers from 11/8/2019
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>new crm, fresh pH cal solutions, new hose for acid dosing</t>
+  </si>
+  <si>
+    <t>crm opened 11/8/2019</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1571,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D62" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D63" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1744,6 +1747,27 @@
       </c>
       <c r="F62" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43781</v>
+      </c>
+      <c r="B63">
+        <v>2147.3009674444802</v>
+      </c>
+      <c r="C63">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="3"/>
+        <v>-2.7063081406016232</v>
+      </c>
+      <c r="E63">
+        <v>169</v>
+      </c>
+      <c r="F63" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second CRM test 11/12/2019 accounting for potentially bad acid influence
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsilbiger\Desktop\Repositories\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\labX_data\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>crm opened 11/8/2019</t>
+  </si>
+  <si>
+    <t>second test run of the day</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,7 +1574,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D63" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D64" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1768,6 +1771,27 @@
       </c>
       <c r="F63" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43781</v>
+      </c>
+      <c r="B64">
+        <v>2212.43486397574</v>
+      </c>
+      <c r="C64">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="3"/>
+        <v>0.24489309052164093</v>
+      </c>
+      <c r="E64">
+        <v>169</v>
+      </c>
+      <c r="F64" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hawaii Samples Run 11/13/2019
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>second test run of the day</t>
+  </si>
+  <si>
+    <t>crm opened 11/8/2019. capped - no evap</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,7 +1577,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D64" si="3">100*(B54-C54)/C54</f>
+        <f t="shared" ref="D54:D65" si="3">100*(B54-C54)/C54</f>
         <v>3.603241658420127</v>
       </c>
       <c r="E54">
@@ -1792,6 +1795,27 @@
       </c>
       <c r="F64" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43782</v>
+      </c>
+      <c r="B65">
+        <v>2211.2751980152798</v>
+      </c>
+      <c r="C65">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="3"/>
+        <v>0.19234890396956922</v>
+      </c>
+      <c r="E65">
+        <v>169</v>
+      </c>
+      <c r="F65" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hawaii Samples 11/19/2019 and 11/20/2019 (last HI Samples)
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>crm opened 11/8/2019. lidded</t>
+  </si>
+  <si>
+    <t>New crm opened 11/19/2019</t>
+  </si>
+  <si>
+    <t>crm opened 11/19/2019</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,6 +1896,48 @@
         <v>31</v>
       </c>
     </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43788</v>
+      </c>
+      <c r="B69">
+        <v>2208.5000007860199</v>
+      </c>
+      <c r="C69">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ref="D69" si="5">100*(B69-C69)/C69</f>
+        <v>6.6605383072259189E-2</v>
+      </c>
+      <c r="E69">
+        <v>169</v>
+      </c>
+      <c r="F69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43789</v>
+      </c>
+      <c r="B70">
+        <v>2203.6505910000001</v>
+      </c>
+      <c r="C70">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D70">
+        <f t="shared" ref="D70" si="6">100*(B70-C70)/C70</f>
+        <v>-0.15312021132472703</v>
+      </c>
+      <c r="E70">
+        <v>169</v>
+      </c>
+      <c r="F70" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Oregon Samples tidepool 13 11/21/2019
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,6 +1938,27 @@
         <v>36</v>
       </c>
     </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43790</v>
+      </c>
+      <c r="B71">
+        <v>2194.45390123274</v>
+      </c>
+      <c r="C71">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D71">
+        <f t="shared" ref="D71" si="7">100*(B71-C71)/C71</f>
+        <v>-0.56982001908719815</v>
+      </c>
+      <c r="E71">
+        <v>169</v>
+      </c>
+      <c r="F71" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tp 14 and 15 samples and sump sample from 11.22
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>crm opened 11/19/2019</t>
+  </si>
+  <si>
+    <t>Crm opened 11/19/2019</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,7 +1952,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D71">
-        <f t="shared" ref="D71" si="7">100*(B71-C71)/C71</f>
+        <f t="shared" ref="D71:D72" si="7">100*(B71-C71)/C71</f>
         <v>-0.56982001908719815</v>
       </c>
       <c r="E71">
@@ -1957,6 +1960,27 @@
       </c>
       <c r="F71" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43791</v>
+      </c>
+      <c r="B72">
+        <v>2189.3936572804901</v>
+      </c>
+      <c r="C72">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="7"/>
+        <v>-0.79909845899286092</v>
+      </c>
+      <c r="E72">
+        <v>169</v>
+      </c>
+      <c r="F72" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tp 16 samples from OR HALF WAY DONE!
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Crm opened 11/19/2019</t>
+  </si>
+  <si>
+    <t>Crm opened 11/19/2020</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,7 +1955,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D71">
-        <f t="shared" ref="D71:D72" si="7">100*(B71-C71)/C71</f>
+        <f t="shared" ref="D71:D76" si="7">100*(B71-C71)/C71</f>
         <v>-0.56982001908719815</v>
       </c>
       <c r="E71">
@@ -1981,6 +1984,45 @@
       </c>
       <c r="F72" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43792</v>
+      </c>
+      <c r="B73">
+        <v>2195.1166635711702</v>
+      </c>
+      <c r="C73">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="7"/>
+        <v>-0.53979041647961312</v>
+      </c>
+      <c r="E73">
+        <v>169</v>
+      </c>
+      <c r="F73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D74" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D75" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D76" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding ocean sample from tp 17-32
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72:F73"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,21 +2008,24 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D74" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D75" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D76" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="A74" s="1">
+        <v>43795</v>
+      </c>
+      <c r="B74">
+        <v>2208.4799460275099</v>
+      </c>
+      <c r="C74">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D74">
+        <f t="shared" ref="D74" si="8">100*(B74-C74)/C74</f>
+        <v>6.5696706773794106E-2</v>
+      </c>
+      <c r="E74">
+        <v>169</v>
+      </c>
+      <c r="F74" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding tp 17 and 18 from OR and edits to HCl
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="C58" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1955,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D71">
-        <f t="shared" ref="D71:D76" si="7">100*(B71-C71)/C71</f>
+        <f t="shared" ref="D71:D73" si="7">100*(B71-C71)/C71</f>
         <v>-0.56982001908719815</v>
       </c>
       <c r="E71">
@@ -2018,7 +2018,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D74">
-        <f t="shared" ref="D74" si="8">100*(B74-C74)/C74</f>
+        <f t="shared" ref="D74:D75" si="8">100*(B74-C74)/C74</f>
         <v>6.5696706773794106E-2</v>
       </c>
       <c r="E74">
@@ -2026,6 +2026,27 @@
       </c>
       <c r="F74" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>43796</v>
+      </c>
+      <c r="B75">
+        <v>2219.1230041260201</v>
+      </c>
+      <c r="C75">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="8"/>
+        <v>0.54793111675055961</v>
+      </c>
+      <c r="E75">
+        <v>169</v>
+      </c>
+      <c r="F75" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tide pools 19 and 20 from OR
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C58" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75:F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,7 +2018,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D74">
-        <f t="shared" ref="D74:D75" si="8">100*(B74-C74)/C74</f>
+        <f t="shared" ref="D74:D76" si="8">100*(B74-C74)/C74</f>
         <v>6.5696706773794106E-2</v>
       </c>
       <c r="E74">
@@ -2047,6 +2047,27 @@
       </c>
       <c r="F75" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>43805</v>
+      </c>
+      <c r="B76">
+        <v>2206.5185511325199</v>
+      </c>
+      <c r="C76">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="8"/>
+        <v>-2.3173625527534273E-2</v>
+      </c>
+      <c r="E76">
+        <v>169</v>
+      </c>
+      <c r="F76" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oregon Samples TP 21 12/11/2019
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -140,7 +140,7 @@
     <t>Crm opened 11/19/2019</t>
   </si>
   <si>
-    <t>Crm opened 11/19/2020</t>
+    <t>New CRM opened 12/11/2019</t>
   </si>
 </sst>
 </file>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75:F76"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2004,7 @@
         <v>169</v>
       </c>
       <c r="F73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2025,7 +2025,7 @@
         <v>169</v>
       </c>
       <c r="F74" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2067,6 +2067,27 @@
         <v>169</v>
       </c>
       <c r="F76" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>43810</v>
+      </c>
+      <c r="B77">
+        <v>2208.24007259168</v>
+      </c>
+      <c r="C77">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ref="D77" si="9">100*(B77-C77)/C77</f>
+        <v>5.482809892388496E-2</v>
+      </c>
+      <c r="E77">
+        <v>169</v>
+      </c>
+      <c r="F77" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding tp 24 and 25 from Oregon4
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>New CRM opened 12/11/2019</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/11/2020</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/11/2021</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,14 +1934,14 @@
         <v>43789</v>
       </c>
       <c r="B70">
-        <v>2203.6505910000001</v>
+        <v>2203.65059131828</v>
       </c>
       <c r="C70">
         <v>2207.0300000000002</v>
       </c>
       <c r="D70">
         <f t="shared" ref="D70" si="6">100*(B70-C70)/C70</f>
-        <v>-0.15312021132472703</v>
+        <v>-0.15312019690353906</v>
       </c>
       <c r="E70">
         <v>169</v>
@@ -2012,14 +2018,14 @@
         <v>43795</v>
       </c>
       <c r="B74">
-        <v>2208.4799460275099</v>
+        <v>2212.26591164927</v>
       </c>
       <c r="C74">
         <v>2207.0300000000002</v>
       </c>
       <c r="D74">
         <f t="shared" ref="D74:D76" si="8">100*(B74-C74)/C74</f>
-        <v>6.5696706773794106E-2</v>
+        <v>0.23723790112820564</v>
       </c>
       <c r="E74">
         <v>169</v>
@@ -2075,20 +2081,62 @@
         <v>43810</v>
       </c>
       <c r="B77">
-        <v>2208.24007259168</v>
+        <v>2212.0256270018399</v>
       </c>
       <c r="C77">
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77" si="9">100*(B77-C77)/C77</f>
-        <v>5.482809892388496E-2</v>
+        <f t="shared" ref="D77:D79" si="9">100*(B77-C77)/C77</f>
+        <v>0.22635066137930582</v>
       </c>
       <c r="E77">
         <v>169</v>
       </c>
       <c r="F77" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>43811</v>
+      </c>
+      <c r="B78">
+        <v>2207.7382817953599</v>
+      </c>
+      <c r="C78">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="9"/>
+        <v>3.2092078284375526E-2</v>
+      </c>
+      <c r="E78">
+        <v>169</v>
+      </c>
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>43812</v>
+      </c>
+      <c r="B79">
+        <v>2206.6755879355001</v>
+      </c>
+      <c r="C79">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="9"/>
+        <v>-1.605832564578363E-2</v>
+      </c>
+      <c r="E79">
+        <v>169</v>
+      </c>
+      <c r="F79" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding tp 26 and 27 from OR
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>New CRM opened 12/11/2021</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/11/2022</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2090,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D79" si="9">100*(B77-C77)/C77</f>
+        <f t="shared" ref="D77:D80" si="9">100*(B77-C77)/C77</f>
         <v>0.22635066137930582</v>
       </c>
       <c r="E77">
@@ -2137,6 +2140,27 @@
       </c>
       <c r="F79" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>43815</v>
+      </c>
+      <c r="B80">
+        <v>2202.4457071062802</v>
+      </c>
+      <c r="C80">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="9"/>
+        <v>-0.20771321158842315</v>
+      </c>
+      <c r="E80">
+        <v>169</v>
+      </c>
+      <c r="F80" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Tp 28-30 from OR
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>New CRM opened 12/11/2022</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/11/2023</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+      <selection activeCell="F80" sqref="F80:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2090,7 +2093,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D80" si="9">100*(B77-C77)/C77</f>
+        <f t="shared" ref="D77:D81" si="9">100*(B77-C77)/C77</f>
         <v>0.22635066137930582</v>
       </c>
       <c r="E77">
@@ -2161,6 +2164,27 @@
       </c>
       <c r="F80" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>43816</v>
+      </c>
+      <c r="B81">
+        <v>2219.6091874158001</v>
+      </c>
+      <c r="C81">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="9"/>
+        <v>0.56995996501179769</v>
+      </c>
+      <c r="E81">
+        <v>169</v>
+      </c>
+      <c r="F81" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done with first round of OR samplesgit add .git add . tp 31 and 32
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -141,18 +141,6 @@
   </si>
   <si>
     <t>New CRM opened 12/11/2019</t>
-  </si>
-  <si>
-    <t>New CRM opened 12/11/2020</t>
-  </si>
-  <si>
-    <t>New CRM opened 12/11/2021</t>
-  </si>
-  <si>
-    <t>New CRM opened 12/11/2022</t>
-  </si>
-  <si>
-    <t>New CRM opened 12/11/2023</t>
   </si>
 </sst>
 </file>
@@ -474,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80:F81"/>
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2081,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D81" si="9">100*(B77-C77)/C77</f>
+        <f t="shared" ref="D77:D83" si="9">100*(B77-C77)/C77</f>
         <v>0.22635066137930582</v>
       </c>
       <c r="E77">
@@ -2121,7 +2109,7 @@
         <v>169</v>
       </c>
       <c r="F78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2142,7 +2130,7 @@
         <v>169</v>
       </c>
       <c r="F79" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2163,7 +2151,7 @@
         <v>169</v>
       </c>
       <c r="F80" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,7 +2172,49 @@
         <v>169</v>
       </c>
       <c r="F81" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>43816</v>
+      </c>
+      <c r="B82">
+        <v>2203.8582110000002</v>
+      </c>
+      <c r="C82">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="9"/>
+        <v>-0.14371299891709624</v>
+      </c>
+      <c r="E82">
+        <v>169</v>
+      </c>
+      <c r="F82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>43817</v>
+      </c>
+      <c r="B83">
+        <v>2208.9061499999998</v>
+      </c>
+      <c r="C83">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="9"/>
+        <v>8.5007906553132381E-2</v>
+      </c>
+      <c r="E83">
+        <v>169</v>
+      </c>
+      <c r="F83" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reruns from OR tide pools
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>New CRM opened 12/11/2019</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/11/2020</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/11/2021</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2087,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D83" si="9">100*(B77-C77)/C77</f>
+        <f t="shared" ref="D77:D84" si="9">100*(B77-C77)/C77</f>
         <v>0.22635066137930582</v>
       </c>
       <c r="E77">
@@ -2215,6 +2221,32 @@
       </c>
       <c r="F83" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>43818</v>
+      </c>
+      <c r="B84">
+        <v>2203.4753172042001</v>
+      </c>
+      <c r="C84">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="9"/>
+        <v>-0.16106182497746246</v>
+      </c>
+      <c r="E84">
+        <v>169</v>
+      </c>
+      <c r="F84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reruns from OR tide pools day 2
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -141,12 +141,6 @@
   </si>
   <si>
     <t>New CRM opened 12/11/2019</t>
-  </si>
-  <si>
-    <t>New CRM opened 12/11/2020</t>
-  </si>
-  <si>
-    <t>New CRM opened 12/11/2021</t>
   </si>
 </sst>
 </file>
@@ -471,7 +465,7 @@
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2081,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D84" si="9">100*(B77-C77)/C77</f>
+        <f t="shared" ref="D77:D85" si="9">100*(B77-C77)/C77</f>
         <v>0.22635066137930582</v>
       </c>
       <c r="E77">
@@ -2241,12 +2235,28 @@
         <v>169</v>
       </c>
       <c r="F84" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>43819</v>
+      </c>
+      <c r="B85">
+        <v>2196.8988871280399</v>
+      </c>
+      <c r="C85">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="9"/>
+        <v>-0.45903829453882999</v>
+      </c>
+      <c r="E85">
+        <v>169</v>
+      </c>
       <c r="F85" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final reruns for TA samples from OR tide pools
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>New CRM opened 12/11/2019</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/21/2019</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2084,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D85" si="9">100*(B77-C77)/C77</f>
+        <f t="shared" ref="D77:D86" si="9">100*(B77-C77)/C77</f>
         <v>0.22635066137930582</v>
       </c>
       <c r="E77">
@@ -2257,6 +2260,32 @@
       </c>
       <c r="F85" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>43820</v>
+      </c>
+      <c r="B86">
+        <v>2221.4069258804502</v>
+      </c>
+      <c r="C86">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="9"/>
+        <v>0.65141506370325797</v>
+      </c>
+      <c r="E86">
+        <v>169</v>
+      </c>
+      <c r="F86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>2207.0300000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding re reruns first 17 samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>New CRM opened 12/21/2019</t>
+  </si>
+  <si>
+    <t>New CRM opened 12/21/2020</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+      <selection activeCell="F86" sqref="F86:F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,7 +2087,7 @@
         <v>2207.0300000000002</v>
       </c>
       <c r="D77">
-        <f t="shared" ref="D77:D86" si="9">100*(B77-C77)/C77</f>
+        <f t="shared" ref="D77:D87" si="9">100*(B77-C77)/C77</f>
         <v>0.22635066137930582</v>
       </c>
       <c r="E77">
@@ -2284,8 +2287,24 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>43472</v>
+      </c>
+      <c r="B87">
+        <v>2218.3052498533202</v>
+      </c>
       <c r="C87">
         <v>2207.0300000000002</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="9"/>
+        <v>0.51087886677208827</v>
+      </c>
+      <c r="E87">
+        <v>169</v>
+      </c>
+      <c r="F87" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katie Meso TA data up to 2/17/2020
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>CRM opened 1/10/2020 (Dudgeon)</t>
+  </si>
+  <si>
+    <t>CRM opened 2/17/2020 (Silbiger bottle for Dudgeon)</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,7 +2351,7 @@
         <v>2235.0700000000002</v>
       </c>
       <c r="D89">
-        <f t="shared" ref="D89" si="10">100*(B89-C89)/C89</f>
+        <f t="shared" ref="D89:D95" si="10">100*(B89-C89)/C89</f>
         <v>0.30099927318113651</v>
       </c>
       <c r="E89">
@@ -2356,6 +2359,132 @@
       </c>
       <c r="F89" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>43860</v>
+      </c>
+      <c r="B90">
+        <v>2235.9172055679701</v>
+      </c>
+      <c r="C90">
+        <v>2235.0700000000002</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="10"/>
+        <v>3.7905102210218131E-2</v>
+      </c>
+      <c r="E90">
+        <v>155</v>
+      </c>
+      <c r="F90" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>43864</v>
+      </c>
+      <c r="B91">
+        <v>2248.65524442177</v>
+      </c>
+      <c r="C91">
+        <v>2235.0700000000002</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="10"/>
+        <v>0.60782187679893052</v>
+      </c>
+      <c r="E91">
+        <v>155</v>
+      </c>
+      <c r="F91" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>43867</v>
+      </c>
+      <c r="B92">
+        <v>2246.27558568522</v>
+      </c>
+      <c r="C92">
+        <v>2235.0700000000002</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="10"/>
+        <v>0.50135278471009093</v>
+      </c>
+      <c r="E92">
+        <v>155</v>
+      </c>
+      <c r="F92" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>43871</v>
+      </c>
+      <c r="B93">
+        <v>2245.1589170981301</v>
+      </c>
+      <c r="C93">
+        <v>2235.0700000000002</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="10"/>
+        <v>0.45139154917429736</v>
+      </c>
+      <c r="E93">
+        <v>155</v>
+      </c>
+      <c r="F93" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>43874</v>
+      </c>
+      <c r="B94">
+        <v>2241.65662945434</v>
+      </c>
+      <c r="C94">
+        <v>2235.0700000000002</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="10"/>
+        <v>0.29469454891076341</v>
+      </c>
+      <c r="E94">
+        <v>155</v>
+      </c>
+      <c r="F94" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>43878</v>
+      </c>
+      <c r="B95">
+        <v>2217.49579116116</v>
+      </c>
+      <c r="C95">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="10"/>
+        <v>0.47420248755838446</v>
+      </c>
+      <c r="E95">
+        <v>169</v>
+      </c>
+      <c r="F95" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Katie's Meso TA data 2-20-2020
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -480,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,7 +2351,7 @@
         <v>2235.0700000000002</v>
       </c>
       <c r="D89">
-        <f t="shared" ref="D89:D95" si="10">100*(B89-C89)/C89</f>
+        <f t="shared" ref="D89:D96" si="10">100*(B89-C89)/C89</f>
         <v>0.30099927318113651</v>
       </c>
       <c r="E89">
@@ -2484,6 +2484,27 @@
         <v>169</v>
       </c>
       <c r="F95" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>43881</v>
+      </c>
+      <c r="B96">
+        <v>2218.2620126549</v>
+      </c>
+      <c r="C96">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="10"/>
+        <v>0.50891979968100975</v>
+      </c>
+      <c r="E96">
+        <v>169</v>
+      </c>
+      <c r="F96" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
9-15-2020 mesocosm_chiachi titrations (initial and 1 week later)
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>CRM opened 2/17/2020 (Silbiger bottle for Dudgeon)</t>
+  </si>
+  <si>
+    <t>CRM opened 9/15/2020</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,7 +2354,7 @@
         <v>2235.0700000000002</v>
       </c>
       <c r="D89">
-        <f t="shared" ref="D89:D96" si="10">100*(B89-C89)/C89</f>
+        <f t="shared" ref="D89:D98" si="10">100*(B89-C89)/C89</f>
         <v>0.30099927318113651</v>
       </c>
       <c r="E89">
@@ -2506,6 +2509,48 @@
       </c>
       <c r="F96" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>43885</v>
+      </c>
+      <c r="B97">
+        <v>2217.29149784021</v>
+      </c>
+      <c r="C97">
+        <v>2214.7603431623102</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="10"/>
+        <v>0.11428571428571727</v>
+      </c>
+      <c r="E97">
+        <v>169</v>
+      </c>
+      <c r="F97" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>44089</v>
+      </c>
+      <c r="B98">
+        <v>2226.5242913638099</v>
+      </c>
+      <c r="C98">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="10"/>
+        <v>9.2349699650257369E-2</v>
+      </c>
+      <c r="E98">
+        <v>180</v>
+      </c>
+      <c r="F98" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update CRM accuracy file through Dec 2020
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,27 @@
   </si>
   <si>
     <t>CRM opened 9/15/2020</t>
+  </si>
+  <si>
+    <t>CRM opened 11/9/2020</t>
+  </si>
+  <si>
+    <t>re-doing with new CRM</t>
+  </si>
+  <si>
+    <t>CRM opened 11/16/2020</t>
+  </si>
+  <si>
+    <t>maybe too much air in it?</t>
+  </si>
+  <si>
+    <t>CRM opened 12/07/2020</t>
+  </si>
+  <si>
+    <t>CRM opened 12/07/2021</t>
+  </si>
+  <si>
+    <t>CRM opened 12/07/2022</t>
   </si>
 </sst>
 </file>
@@ -483,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,7 +2375,7 @@
         <v>2235.0700000000002</v>
       </c>
       <c r="D89">
-        <f t="shared" ref="D89:D98" si="10">100*(B89-C89)/C89</f>
+        <f t="shared" ref="D89:D97" si="10">100*(B89-C89)/C89</f>
         <v>0.30099927318113651</v>
       </c>
       <c r="E89">
@@ -2511,7 +2532,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43885</v>
       </c>
@@ -2532,7 +2553,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44089</v>
       </c>
@@ -2543,7 +2564,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D98">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D98:D107" si="11">100*(B98-C98)/C98</f>
         <v>9.2349699650257369E-2</v>
       </c>
       <c r="E98">
@@ -2551,6 +2572,198 @@
       </c>
       <c r="F98" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>44099</v>
+      </c>
+      <c r="B99">
+        <v>2223.85573616478</v>
+      </c>
+      <c r="C99">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="11"/>
+        <v>-2.7613941083487064E-2</v>
+      </c>
+      <c r="E99">
+        <v>180</v>
+      </c>
+      <c r="F99" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>44144</v>
+      </c>
+      <c r="B100">
+        <v>2225.0953859339002</v>
+      </c>
+      <c r="C100">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="11"/>
+        <v>2.8113929785538182E-2</v>
+      </c>
+      <c r="E100">
+        <v>180</v>
+      </c>
+      <c r="F100" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>44151</v>
+      </c>
+      <c r="B101">
+        <v>2192.2550000000001</v>
+      </c>
+      <c r="C101">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="11"/>
+        <v>-1.4482101354479806</v>
+      </c>
+      <c r="E101">
+        <v>180</v>
+      </c>
+      <c r="F101" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>44151</v>
+      </c>
+      <c r="B102">
+        <v>2196.7869999999998</v>
+      </c>
+      <c r="C102">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="11"/>
+        <v>-1.2444762123112469</v>
+      </c>
+      <c r="E102">
+        <v>180</v>
+      </c>
+      <c r="F102" t="s">
+        <v>48</v>
+      </c>
+      <c r="G102" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>44151</v>
+      </c>
+      <c r="B103">
+        <v>2210.4760000000001</v>
+      </c>
+      <c r="C103">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="11"/>
+        <v>-0.62909367175100983</v>
+      </c>
+      <c r="E103">
+        <v>180</v>
+      </c>
+      <c r="F103" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B104">
+        <v>2229.54539136422</v>
+      </c>
+      <c r="C104">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="11"/>
+        <v>0.22816182570321</v>
+      </c>
+      <c r="E104">
+        <v>180</v>
+      </c>
+      <c r="F104" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>44172</v>
+      </c>
+      <c r="B105">
+        <v>2216.68934643902</v>
+      </c>
+      <c r="C105">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="11"/>
+        <v>-0.34977561221233699</v>
+      </c>
+      <c r="E105">
+        <v>180</v>
+      </c>
+      <c r="F105" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>44181</v>
+      </c>
+      <c r="B106">
+        <v>2205.9340000000002</v>
+      </c>
+      <c r="C106">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="11"/>
+        <v>-0.83327714017269749</v>
+      </c>
+      <c r="E106">
+        <v>180</v>
+      </c>
+      <c r="F106" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>44194</v>
+      </c>
+      <c r="B107">
+        <v>2208.1210672914899</v>
+      </c>
+      <c r="C107">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="11"/>
+        <v>-0.73495856129819204</v>
+      </c>
+      <c r="E107">
+        <v>180</v>
+      </c>
+      <c r="F107" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test runs sept 1-3. Update script to install old seacarb package version
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -510,7 +510,7 @@
   <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,7 +2567,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D98">
-        <f t="shared" ref="D98:D107" si="11">100*(B98-C98)/C98</f>
+        <f t="shared" ref="D98:D108" si="11">100*(B98-C98)/C98</f>
         <v>9.2349699650257369E-2</v>
       </c>
       <c r="E98">
@@ -2773,8 +2773,15 @@
       <c r="A108" s="1">
         <v>44440</v>
       </c>
+      <c r="B108">
+        <v>2118.7343673246701</v>
+      </c>
       <c r="C108">
         <v>2230.52</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="11"/>
+        <v>-5.0116400066051821</v>
       </c>
       <c r="E108">
         <v>183</v>

</xml_diff>

<commit_message>
new crm run after titrant change
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>CRM opened 9/1/2021</t>
+  </si>
+  <si>
+    <t>CRM opened 9/1/2021; new titrant opened 9/7/2021</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2790,6 +2793,27 @@
         <v>53</v>
       </c>
     </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>44446</v>
+      </c>
+      <c r="B109">
+        <v>2231.6853052162301</v>
+      </c>
+      <c r="C109">
+        <v>2230.52</v>
+      </c>
+      <c r="D109">
+        <f t="shared" ref="D109" si="12">100*(B109-C109)/C109</f>
+        <v>5.2243656915431425E-2</v>
+      </c>
+      <c r="E109">
+        <v>183</v>
+      </c>
+      <c r="F109" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Titration documents added for first set of 30 samples, 9/16/2021
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -513,10 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E112" sqref="E112:F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,13 +2829,55 @@
         <v>2230.52</v>
       </c>
       <c r="D110">
-        <f t="shared" ref="D110" si="13">100*(B110-C110)/C110</f>
+        <f t="shared" ref="D110:D112" si="13">100*(B110-C110)/C110</f>
         <v>0.27273229817934763</v>
       </c>
       <c r="E110">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F110" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>44454</v>
+      </c>
+      <c r="B111">
+        <v>2247.3113498889102</v>
+      </c>
+      <c r="C111">
+        <v>2230.52</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="13"/>
+        <v>0.7527997905829219</v>
+      </c>
+      <c r="E111">
+        <v>183</v>
+      </c>
+      <c r="F111" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B112">
+        <v>2238.5667683911502</v>
+      </c>
+      <c r="C112">
+        <v>2230.52</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="13"/>
+        <v>0.3607575090629172</v>
+      </c>
+      <c r="E112">
+        <v>183</v>
+      </c>
+      <c r="F112" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sept 20 & 21 titration data folders
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -513,11 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2829,7 +2829,7 @@
         <v>2230.52</v>
       </c>
       <c r="D110">
-        <f t="shared" ref="D110:D113" si="13">100*(B110-C110)/C110</f>
+        <f t="shared" ref="D110:D115" si="13">100*(B110-C110)/C110</f>
         <v>0.27273229817934763</v>
       </c>
       <c r="E110">
@@ -2899,6 +2899,48 @@
         <v>183</v>
       </c>
       <c r="F113" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B114">
+        <v>2238.28837133754</v>
+      </c>
+      <c r="C114">
+        <v>2230.52</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="13"/>
+        <v>0.34827624668418011</v>
+      </c>
+      <c r="E114">
+        <v>183</v>
+      </c>
+      <c r="F114" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>44460</v>
+      </c>
+      <c r="B115">
+        <v>2245.6299964466002</v>
+      </c>
+      <c r="C115">
+        <v>2230.52</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="13"/>
+        <v>0.6774203525007727</v>
+      </c>
+      <c r="E115">
+        <v>183</v>
+      </c>
+      <c r="F115" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sept 22 titrator sample files added
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -513,11 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2944,6 +2944,27 @@
         <v>55</v>
       </c>
     </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>44461</v>
+      </c>
+      <c r="B116">
+        <v>2244.40054141874</v>
+      </c>
+      <c r="C116">
+        <v>2230.52</v>
+      </c>
+      <c r="D116">
+        <f t="shared" ref="D116" si="14">100*(B116-C116)/C116</f>
+        <v>0.62230069305543079</v>
+      </c>
+      <c r="E116">
+        <v>183</v>
+      </c>
+      <c r="F116" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
water sampling titrations 9/27/2021
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -519,11 +519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F120" sqref="F120"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2961,7 +2961,7 @@
         <v>2230.52</v>
       </c>
       <c r="D116">
-        <f t="shared" ref="D116:D118" si="14">100*(B116-C116)/C116</f>
+        <f t="shared" ref="D116:D120" si="14">100*(B116-C116)/C116</f>
         <v>0.62230069305543079</v>
       </c>
       <c r="E116">
@@ -3014,7 +3014,46 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
+      <c r="A119" s="1">
+        <v>44466</v>
+      </c>
+      <c r="B119">
+        <v>2265.0046219237502</v>
+      </c>
+      <c r="C119">
+        <v>2230.52</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="14"/>
+        <v>1.5460350915369592</v>
+      </c>
+      <c r="E119">
+        <v>183</v>
+      </c>
+      <c r="F119" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>44466</v>
+      </c>
+      <c r="B120">
+        <v>2245.7404688474599</v>
+      </c>
+      <c r="C120">
+        <v>2230.52</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="14"/>
+        <v>0.68237311691712554</v>
+      </c>
+      <c r="E120">
+        <v>183</v>
+      </c>
+      <c r="F120" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sample titrations from 9/29/2021
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>CRM opened 9/24/2021</t>
+  </si>
+  <si>
+    <t>CRM opened 9/29/2021</t>
   </si>
 </sst>
 </file>
@@ -519,11 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3055,6 +3058,48 @@
         <v>57</v>
       </c>
     </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>44467</v>
+      </c>
+      <c r="B121">
+        <v>2250.79045167291</v>
+      </c>
+      <c r="C121">
+        <v>2230.52</v>
+      </c>
+      <c r="D121">
+        <f>100*(B121-C121)/C121</f>
+        <v>0.90877695214165244</v>
+      </c>
+      <c r="E121">
+        <v>183</v>
+      </c>
+      <c r="F121" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>44468</v>
+      </c>
+      <c r="B122">
+        <v>2249.1843699999999</v>
+      </c>
+      <c r="C122">
+        <v>2230.52</v>
+      </c>
+      <c r="D122">
+        <f>100*(B122-C122)/C122</f>
+        <v>0.83677214281871326</v>
+      </c>
+      <c r="E122">
+        <v>191</v>
+      </c>
+      <c r="F122" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
updated titration data 9/29/2021
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -525,8 +525,8 @@
   <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Putnam Lab Moorea Sample Titration 2021_10_08
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>CRM opened 9/24/2021</t>
+  </si>
+  <si>
+    <t>CRM opened 9/29/2021 (titrations were run - CRM value was previously compared to batch 183 value and showed &lt;1% error)</t>
   </si>
   <si>
     <t>CRM opened 9/29/2021</t>
@@ -522,11 +525,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F126" sqref="F126"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,17 +3090,59 @@
         <v>2249.1843699999999</v>
       </c>
       <c r="C122">
-        <v>2230.52</v>
+        <v>2225.5</v>
       </c>
       <c r="D122">
         <f>100*(B122-C122)/C122</f>
-        <v>0.83677214281871326</v>
+        <v>1.0642269152999302</v>
       </c>
       <c r="E122">
         <v>191</v>
       </c>
       <c r="F122" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>44474</v>
+      </c>
+      <c r="B123">
+        <v>2243.9480014356</v>
+      </c>
+      <c r="C123">
+        <v>2230.52</v>
+      </c>
+      <c r="D123">
+        <f>100*(B123-C123)/C123</f>
+        <v>0.60201215122930896</v>
+      </c>
+      <c r="E123">
+        <v>183</v>
+      </c>
+      <c r="F123" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>44477</v>
+      </c>
+      <c r="B124">
+        <v>2238.29693071969</v>
+      </c>
+      <c r="C124">
+        <v>2225.5</v>
+      </c>
+      <c r="D124">
+        <f>100*(B124-C124)/C124</f>
+        <v>0.57501373712379034</v>
+      </c>
+      <c r="E124">
+        <v>191</v>
+      </c>
+      <c r="F124" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last two runs of Putnam sample TAs
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -204,19 +204,28 @@
   </si>
   <si>
     <t>CRM opened 9/29/2021</t>
+  </si>
+  <si>
+    <t>CRM opened 10/20/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -239,12 +248,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D126" sqref="D126"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,6 +3155,48 @@
         <v>59</v>
       </c>
     </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>44484</v>
+      </c>
+      <c r="B125">
+        <v>2213.7399999999998</v>
+      </c>
+      <c r="C125">
+        <v>2225.5</v>
+      </c>
+      <c r="D125">
+        <f>100*(B125-C125)/C125</f>
+        <v>-0.52842057964503342</v>
+      </c>
+      <c r="E125">
+        <v>191</v>
+      </c>
+      <c r="F125" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>44489</v>
+      </c>
+      <c r="B126">
+        <v>2230.9353385324998</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D126">
+        <f>100*(B126-C126)/C126</f>
+        <v>0.29064624528539507</v>
+      </c>
+      <c r="E126">
+        <v>180</v>
+      </c>
+      <c r="F126" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adding High Night water samples from mar 2022
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>CRM opened 10/20/2021</t>
+  </si>
+  <si>
+    <t>CRM opened 12/14/2021</t>
   </si>
 </sst>
 </file>
@@ -535,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G127" sqref="G127"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3082,7 +3085,7 @@
         <v>2230.52</v>
       </c>
       <c r="D121">
-        <f>100*(B121-C121)/C121</f>
+        <f t="shared" ref="D121:D126" si="15">100*(B121-C121)/C121</f>
         <v>0.90877695214165244</v>
       </c>
       <c r="E121">
@@ -3103,7 +3106,7 @@
         <v>2225.5</v>
       </c>
       <c r="D122">
-        <f>100*(B122-C122)/C122</f>
+        <f t="shared" si="15"/>
         <v>1.0642269152999302</v>
       </c>
       <c r="E122">
@@ -3124,7 +3127,7 @@
         <v>2230.52</v>
       </c>
       <c r="D123">
-        <f>100*(B123-C123)/C123</f>
+        <f t="shared" si="15"/>
         <v>0.60201215122930896</v>
       </c>
       <c r="E123">
@@ -3145,7 +3148,7 @@
         <v>2225.5</v>
       </c>
       <c r="D124">
-        <f>100*(B124-C124)/C124</f>
+        <f t="shared" si="15"/>
         <v>0.57501373712379034</v>
       </c>
       <c r="E124">
@@ -3166,7 +3169,7 @@
         <v>2225.5</v>
       </c>
       <c r="D125">
-        <f>100*(B125-C125)/C125</f>
+        <f t="shared" si="15"/>
         <v>-0.52842057964503342</v>
       </c>
       <c r="E125">
@@ -3187,7 +3190,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D126">
-        <f>100*(B126-C126)/C126</f>
+        <f t="shared" si="15"/>
         <v>0.29064624528539507</v>
       </c>
       <c r="E126">
@@ -3195,6 +3198,48 @@
       </c>
       <c r="F126" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>44544</v>
+      </c>
+      <c r="B127">
+        <v>2229.0967744312802</v>
+      </c>
+      <c r="C127" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D127">
+        <f>100*(B127-C127)/C127</f>
+        <v>0.20799446300828558</v>
+      </c>
+      <c r="E127">
+        <v>180</v>
+      </c>
+      <c r="F127" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>44656</v>
+      </c>
+      <c r="B128">
+        <v>2234.7794657772101</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D128">
+        <f>100*(B128-C128)/C128</f>
+        <v>0.46345717304393114</v>
+      </c>
+      <c r="E128">
+        <v>180</v>
+      </c>
+      <c r="F128" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Virari Seep and Low Night samples Moorea March 2022
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -538,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A135" sqref="A135"/>
+      <selection pane="bottomLeft" activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,6 +3242,27 @@
         <v>61</v>
       </c>
     </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>44657</v>
+      </c>
+      <c r="B129">
+        <v>2233.20682882136</v>
+      </c>
+      <c r="C129" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D129">
+        <f>100*(B129-C129)/C129</f>
+        <v>0.39276002020077494</v>
+      </c>
+      <c r="E129">
+        <v>180</v>
+      </c>
+      <c r="F129" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adding crm for april 7th
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>CRM opened 12/14/2021</t>
+  </si>
+  <si>
+    <t>CRM opened 4/7/2022</t>
   </si>
 </sst>
 </file>
@@ -538,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F129" sqref="F129"/>
+      <selection pane="bottomLeft" activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,6 +3266,27 @@
         <v>61</v>
       </c>
     </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>44658</v>
+      </c>
+      <c r="B130">
+        <v>2238.6216475053602</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D130">
+        <f>100*(B130-C130)/C130</f>
+        <v>0.63618064102282412</v>
+      </c>
+      <c r="E130">
+        <v>180</v>
+      </c>
+      <c r="F130" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
04082022 reefcrest TA samples March 2022
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F131" sqref="F131"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F132" sqref="F132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,6 +3287,27 @@
         <v>62</v>
       </c>
     </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>44659</v>
+      </c>
+      <c r="B131">
+        <v>2235.0609128819601</v>
+      </c>
+      <c r="C131" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D131">
+        <f>100*(B131-C131)/C131</f>
+        <v>0.47610949493408866</v>
+      </c>
+      <c r="E131">
+        <v>180</v>
+      </c>
+      <c r="F131" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
adding cabral high night samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F132" sqref="F132"/>
+      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,6 +3308,27 @@
         <v>62</v>
       </c>
     </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>44662</v>
+      </c>
+      <c r="B132">
+        <v>2237.58134409885</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D132">
+        <f>100*(B132-C132)/C132</f>
+        <v>0.58941429189200889</v>
+      </c>
+      <c r="E132">
+        <v>180</v>
+      </c>
+      <c r="F132" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Cabral Seeps and Low Night samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -541,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <selection pane="bottomLeft" activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3214,7 +3214,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D127">
-        <f>100*(B127-C127)/C127</f>
+        <f t="shared" ref="D127:D133" si="16">100*(B127-C127)/C127</f>
         <v>0.20799446300828558</v>
       </c>
       <c r="E127">
@@ -3235,7 +3235,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D128">
-        <f>100*(B128-C128)/C128</f>
+        <f t="shared" si="16"/>
         <v>0.46345717304393114</v>
       </c>
       <c r="E128">
@@ -3256,7 +3256,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D129">
-        <f>100*(B129-C129)/C129</f>
+        <f t="shared" si="16"/>
         <v>0.39276002020077494</v>
       </c>
       <c r="E129">
@@ -3277,7 +3277,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D130">
-        <f>100*(B130-C130)/C130</f>
+        <f t="shared" si="16"/>
         <v>0.63618064102282412</v>
       </c>
       <c r="E130">
@@ -3298,7 +3298,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D131">
-        <f>100*(B131-C131)/C131</f>
+        <f t="shared" si="16"/>
         <v>0.47610949493408866</v>
       </c>
       <c r="E131">
@@ -3319,13 +3319,34 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D132">
-        <f>100*(B132-C132)/C132</f>
+        <f t="shared" si="16"/>
         <v>0.58941429189200889</v>
       </c>
       <c r="E132">
         <v>180</v>
       </c>
       <c r="F132" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>44663</v>
+      </c>
+      <c r="B133">
+        <v>2234.5838387866102</v>
+      </c>
+      <c r="C133" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="16"/>
+        <v>0.45466285392072536</v>
+      </c>
+      <c r="E133">
+        <v>180</v>
+      </c>
+      <c r="F133" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding rerun cabral reef crests, c pit samples, and c bottoms
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>CRM opened 4/7/2022</t>
+  </si>
+  <si>
+    <t>New CRM open 4/15/2022</t>
   </si>
 </sst>
 </file>
@@ -254,13 +257,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +547,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
@@ -3214,7 +3220,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D127">
-        <f t="shared" ref="D127:D133" si="16">100*(B127-C127)/C127</f>
+        <f t="shared" ref="D127:D134" si="16">100*(B127-C127)/C127</f>
         <v>0.20799446300828558</v>
       </c>
       <c r="E127">
@@ -3348,6 +3354,32 @@
       </c>
       <c r="F133" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>44665</v>
+      </c>
+      <c r="B134">
+        <v>2234.9628598622999</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="16"/>
+        <v>0.47170156766780702</v>
+      </c>
+      <c r="E134" s="4">
+        <v>180</v>
+      </c>
+      <c r="F134" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F135" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding samples from cabral high day
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -551,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E134" sqref="E134"/>
+      <selection pane="bottomLeft" activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3220,7 +3220,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D127">
-        <f t="shared" ref="D127:D134" si="16">100*(B127-C127)/C127</f>
+        <f t="shared" ref="D127:D135" si="16">100*(B127-C127)/C127</f>
         <v>0.20799446300828558</v>
       </c>
       <c r="E127">
@@ -3378,6 +3378,22 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>44666</v>
+      </c>
+      <c r="B135">
+        <v>2246.14693334713</v>
+      </c>
+      <c r="C135">
+        <v>2230.52</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="16"/>
+        <v>0.70059597524927075</v>
+      </c>
+      <c r="E135">
+        <v>183</v>
+      </c>
       <c r="F135" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
adding varari wells from Aug 2022
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>New CRM open 4/15/2022</t>
+  </si>
+  <si>
+    <t>CRM open 4/15/2022</t>
   </si>
 </sst>
 </file>
@@ -547,11 +550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F136" sqref="F136"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3220,7 +3223,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D127">
-        <f t="shared" ref="D127:D136" si="16">100*(B127-C127)/C127</f>
+        <f t="shared" ref="D127:D137" si="16">100*(B127-C127)/C127</f>
         <v>0.20799446300828558</v>
       </c>
       <c r="E127">
@@ -3417,6 +3420,27 @@
       </c>
       <c r="F136" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>44697</v>
+      </c>
+      <c r="B137">
+        <v>2219.1097641833899</v>
+      </c>
+      <c r="C137">
+        <v>2230.52</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="16"/>
+        <v>-0.51155048224674571</v>
+      </c>
+      <c r="E137">
+        <v>183</v>
+      </c>
+      <c r="F137" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding CRM accurancy after run
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>CRM opened 6/2/2022</t>
+  </si>
+  <si>
+    <t>after 33 samples; CRM opened 6/2/2022</t>
   </si>
 </sst>
 </file>
@@ -555,9 +558,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
+      <selection pane="bottomLeft" activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,7 +3488,7 @@
         <v>191</v>
       </c>
       <c r="F139" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new data from August 2023 test
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t>CRM opened 8/21/2022</t>
+  </si>
+  <si>
+    <t>New CRM opened 8/27/2022</t>
+  </si>
+  <si>
+    <t>CRM opened 8/27/2022</t>
+  </si>
+  <si>
+    <t>CRM opened 11/17/2022</t>
+  </si>
+  <si>
+    <t>CRM opened 2022-12-13</t>
+  </si>
+  <si>
+    <t>CRM opened 2022-12-21</t>
+  </si>
+  <si>
+    <t>CRM opened 4/4/2023</t>
   </si>
 </sst>
 </file>
@@ -559,11 +577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A142" sqref="A142:F142"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,7 +3250,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D127">
-        <f t="shared" ref="D127:D142" si="16">100*(B127-C127)/C127</f>
+        <f t="shared" ref="D127:D140" si="16">100*(B127-C127)/C127</f>
         <v>0.20799446300828558</v>
       </c>
       <c r="E127">
@@ -3526,7 +3544,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D141">
-        <f t="shared" ref="D141" si="17">100*(B141-C141)/C141</f>
+        <f t="shared" ref="D141:D162" si="17">100*(B141-C141)/C141</f>
         <v>-0.99218103628862764</v>
       </c>
       <c r="E141">
@@ -3537,8 +3555,442 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
-      <c r="C142" s="3"/>
+      <c r="A142" s="1">
+        <v>44800</v>
+      </c>
+      <c r="B142">
+        <v>2252.4587351766299</v>
+      </c>
+      <c r="C142">
+        <v>2225.5</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="17"/>
+        <v>1.2113563323581191</v>
+      </c>
+      <c r="E142">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>44800</v>
+      </c>
+      <c r="B143">
+        <v>2249.5919395711398</v>
+      </c>
+      <c r="C143" s="3">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="17"/>
+        <v>1.1293449482861109</v>
+      </c>
+      <c r="E143">
+        <v>180</v>
+      </c>
+      <c r="F143" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>44800</v>
+      </c>
+      <c r="B144">
+        <v>2229.9277457974299</v>
+      </c>
+      <c r="C144">
+        <v>2230.52</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="17"/>
+        <v>-2.6552292854136031E-2</v>
+      </c>
+      <c r="E144">
+        <v>183</v>
+      </c>
+      <c r="F144" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>44803</v>
+      </c>
+      <c r="B145">
+        <v>2232.5404066472402</v>
+      </c>
+      <c r="C145">
+        <v>2230.52</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="17"/>
+        <v>9.0580073132730449E-2</v>
+      </c>
+      <c r="E145">
+        <v>183</v>
+      </c>
+      <c r="F145" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B146">
+        <v>2246.7591080000002</v>
+      </c>
+      <c r="C146">
+        <v>2230.52</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="17"/>
+        <v>0.72804135358572064</v>
+      </c>
+      <c r="E146">
+        <v>183</v>
+      </c>
+      <c r="F146" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>44882</v>
+      </c>
+      <c r="B147">
+        <v>2251.5197182939401</v>
+      </c>
+      <c r="C147" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="17"/>
+        <v>1.1691628080853766</v>
+      </c>
+      <c r="E147">
+        <v>191</v>
+      </c>
+      <c r="F147" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>44882</v>
+      </c>
+      <c r="B148">
+        <v>2247.6284427516698</v>
+      </c>
+      <c r="C148" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="17"/>
+        <v>0.99431331169039805</v>
+      </c>
+      <c r="E148">
+        <v>191</v>
+      </c>
+      <c r="F148" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>44882</v>
+      </c>
+      <c r="B149">
+        <v>2236.2906877866599</v>
+      </c>
+      <c r="C149" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="17"/>
+        <v>0.48486577338395298</v>
+      </c>
+      <c r="E149">
+        <v>191</v>
+      </c>
+      <c r="F149" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>44882</v>
+      </c>
+      <c r="B150">
+        <v>2221.0105802766798</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="17"/>
+        <v>-0.2017263411961458</v>
+      </c>
+      <c r="E150">
+        <v>191</v>
+      </c>
+      <c r="F150" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>44883</v>
+      </c>
+      <c r="B151">
+        <v>2240.1143773028998</v>
+      </c>
+      <c r="C151" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="17"/>
+        <v>0.65667837802290774</v>
+      </c>
+      <c r="E151">
+        <v>191</v>
+      </c>
+      <c r="F151" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>44908</v>
+      </c>
+      <c r="B152">
+        <v>2253.5423536174399</v>
+      </c>
+      <c r="C152" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="17"/>
+        <v>1.2600473429539365</v>
+      </c>
+      <c r="E152">
+        <v>191</v>
+      </c>
+      <c r="F152" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>44908</v>
+      </c>
+      <c r="B153">
+        <v>2248.8867845742002</v>
+      </c>
+      <c r="C153" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D153">
+        <f t="shared" si="17"/>
+        <v>1.0508552942799456</v>
+      </c>
+      <c r="E153">
+        <v>191</v>
+      </c>
+      <c r="F153" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>44908</v>
+      </c>
+      <c r="B154">
+        <v>2223.8078839847099</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D154">
+        <f t="shared" si="17"/>
+        <v>-7.603307190699346E-2</v>
+      </c>
+      <c r="E154">
+        <v>191</v>
+      </c>
+      <c r="F154" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>44910</v>
+      </c>
+      <c r="B155">
+        <v>2236.8053891996001</v>
+      </c>
+      <c r="C155" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D155">
+        <f t="shared" si="17"/>
+        <v>0.50799322397663826</v>
+      </c>
+      <c r="E155">
+        <v>191</v>
+      </c>
+      <c r="F155" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>44911</v>
+      </c>
+      <c r="B156">
+        <v>2240.1060148698698</v>
+      </c>
+      <c r="C156" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D156">
+        <f t="shared" si="17"/>
+        <v>0.65630262277554685</v>
+      </c>
+      <c r="E156">
+        <v>191</v>
+      </c>
+      <c r="F156" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>44914</v>
+      </c>
+      <c r="B157">
+        <v>2224.52623796326</v>
+      </c>
+      <c r="C157" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D157">
+        <f t="shared" si="17"/>
+        <v>-4.3754753392047936E-2</v>
+      </c>
+      <c r="E157">
+        <v>191</v>
+      </c>
+      <c r="F157" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>44915</v>
+      </c>
+      <c r="B158">
+        <v>2249.06168130893</v>
+      </c>
+      <c r="C158" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D158">
+        <f t="shared" si="17"/>
+        <v>1.0587140556697381</v>
+      </c>
+      <c r="E158">
+        <v>191</v>
+      </c>
+      <c r="F158" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>44915</v>
+      </c>
+      <c r="B159">
+        <v>2232.1446972612798</v>
+      </c>
+      <c r="C159" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D159">
+        <f t="shared" si="17"/>
+        <v>0.29857098455537256</v>
+      </c>
+      <c r="E159">
+        <v>191</v>
+      </c>
+      <c r="F159" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>44916</v>
+      </c>
+      <c r="B160">
+        <v>2222.9937336656999</v>
+      </c>
+      <c r="C160" s="3">
+        <v>2225.5</v>
+      </c>
+      <c r="D160">
+        <f t="shared" si="17"/>
+        <v>-0.11261587662548227</v>
+      </c>
+      <c r="E160">
+        <v>191</v>
+      </c>
+      <c r="F160" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>45021</v>
+      </c>
+      <c r="B161">
+        <v>2202.2406761348202</v>
+      </c>
+      <c r="C161" s="3">
+        <v>2215.13</v>
+      </c>
+      <c r="D161">
+        <f t="shared" si="17"/>
+        <v>-0.58187663320797889</v>
+      </c>
+      <c r="E161">
+        <v>202</v>
+      </c>
+      <c r="F161" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>45022</v>
+      </c>
+      <c r="B162">
+        <v>2230.1596600173102</v>
+      </c>
+      <c r="C162" s="3">
+        <v>2215.13</v>
+      </c>
+      <c r="D162">
+        <f t="shared" si="17"/>
+        <v>0.6785001339564769</v>
+      </c>
+      <c r="E162">
+        <v>202</v>
+      </c>
+      <c r="F162" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
push the last 7 months of data
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -247,13 +247,43 @@
   </si>
   <si>
     <t>CRM opened 08/16/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 8/31/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 9/7/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 9/15/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 9/20/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 9/22/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 10/03/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 11/16/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 11/29/2023</t>
+  </si>
+  <si>
+    <t>CRM opened 1/4/2024</t>
+  </si>
+  <si>
+    <t>CRM opened 2/28/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +417,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -730,9 +772,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1054,11 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F171" sqref="F171"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A235" sqref="A235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,6 +1111,7 @@
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4415,17 +4460,14 @@
         <v>2203</v>
       </c>
       <c r="C168">
-        <v>2199.3200000000002</v>
+        <v>2225.5</v>
       </c>
       <c r="D168">
         <f>100*(B168-C168)/C168</f>
-        <v>0.16732444573776603</v>
+        <v>-1.011008762075938</v>
       </c>
       <c r="E168">
-        <v>207</v>
-      </c>
-      <c r="F168" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -4436,17 +4478,14 @@
         <v>2194.6772531250899</v>
       </c>
       <c r="C169">
-        <v>2199.3200000000002</v>
+        <v>2225.5</v>
       </c>
       <c r="D169">
         <f>100*(B169-C169)/C169</f>
-        <v>-0.21109919770248278</v>
+        <v>-1.3849807627459034</v>
       </c>
       <c r="E169">
-        <v>207</v>
-      </c>
-      <c r="F169" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -4470,7 +4509,1343 @@
         <v>75</v>
       </c>
     </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>45163</v>
+      </c>
+      <c r="B171">
+        <v>2193.7730799999999</v>
+      </c>
+      <c r="C171">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D171">
+        <f t="shared" ref="D171:D196" si="0">100*(B171-C171)/C171</f>
+        <v>-0.25221068330212187</v>
+      </c>
+      <c r="E171">
+        <v>207</v>
+      </c>
+      <c r="F171" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>45166</v>
+      </c>
+      <c r="B172">
+        <v>2184.25952148239</v>
+      </c>
+      <c r="C172">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D172">
+        <f t="shared" si="0"/>
+        <v>-0.68477886426759793</v>
+      </c>
+      <c r="E172">
+        <v>207</v>
+      </c>
+      <c r="F172" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B173">
+        <v>2211.2263493318601</v>
+      </c>
+      <c r="C173">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D173">
+        <f>100*(B173-C173)/C173</f>
+        <v>0.5413650279113511</v>
+      </c>
+      <c r="E173">
+        <v>207</v>
+      </c>
+      <c r="F173" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B174">
+        <v>2216.46092967194</v>
+      </c>
+      <c r="C174">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D174">
+        <f t="shared" si="0"/>
+        <v>0.77937406434442591</v>
+      </c>
+      <c r="E174">
+        <v>207</v>
+      </c>
+      <c r="F174" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B175">
+        <v>2207.6704806037801</v>
+      </c>
+      <c r="C175">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D175">
+        <f t="shared" si="0"/>
+        <v>0.37968465724769213</v>
+      </c>
+      <c r="E175">
+        <v>207</v>
+      </c>
+      <c r="F175" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>45174</v>
+      </c>
+      <c r="B176">
+        <v>2214.04637</v>
+      </c>
+      <c r="C176">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D176">
+        <f t="shared" si="0"/>
+        <v>0.66958741792917176</v>
+      </c>
+      <c r="E176">
+        <v>207</v>
+      </c>
+      <c r="F176" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>45176</v>
+      </c>
+      <c r="B177">
+        <v>2215.1709401202302</v>
+      </c>
+      <c r="C177">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D177">
+        <f t="shared" si="0"/>
+        <v>0.72072004620655505</v>
+      </c>
+      <c r="E177">
+        <v>207</v>
+      </c>
+      <c r="F177" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>45177</v>
+      </c>
+      <c r="B178" s="2">
+        <v>2218.4690000000001</v>
+      </c>
+      <c r="C178">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D178">
+        <f t="shared" si="0"/>
+        <v>0.87067820962842546</v>
+      </c>
+      <c r="E178">
+        <v>207</v>
+      </c>
+      <c r="F178" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>45180</v>
+      </c>
+      <c r="B179">
+        <v>2212.9283429509901</v>
+      </c>
+      <c r="C179">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D179">
+        <f t="shared" si="0"/>
+        <v>0.61875229393584996</v>
+      </c>
+      <c r="E179">
+        <v>207</v>
+      </c>
+      <c r="F179" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>45181</v>
+      </c>
+      <c r="B180">
+        <v>2217.71213828707</v>
+      </c>
+      <c r="C180">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D180">
+        <f t="shared" si="0"/>
+        <v>0.83626476761316604</v>
+      </c>
+      <c r="E180">
+        <v>207</v>
+      </c>
+      <c r="F180" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>45182</v>
+      </c>
+      <c r="B181">
+        <v>2213.1445675301202</v>
+      </c>
+      <c r="C181">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D181">
+        <f t="shared" si="0"/>
+        <v>0.62858372270156315</v>
+      </c>
+      <c r="E181">
+        <v>207</v>
+      </c>
+      <c r="F181" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>45183</v>
+      </c>
+      <c r="B182">
+        <v>2219.8148046501601</v>
+      </c>
+      <c r="C182">
+        <v>2199.3200000000002</v>
+      </c>
+      <c r="D182">
+        <f t="shared" si="0"/>
+        <v>0.93187006211737933</v>
+      </c>
+      <c r="E182">
+        <v>207</v>
+      </c>
+      <c r="F182" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>45184</v>
+      </c>
+      <c r="B183">
+        <v>2222.8246917193601</v>
+      </c>
+      <c r="C183">
+        <v>2215.13</v>
+      </c>
+      <c r="D183">
+        <f t="shared" si="0"/>
+        <v>0.34736975795370834</v>
+      </c>
+      <c r="E183">
+        <v>202</v>
+      </c>
+      <c r="F183" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>45187</v>
+      </c>
+      <c r="B184">
+        <v>2249.3352644462602</v>
+      </c>
+      <c r="C184">
+        <v>2215.13</v>
+      </c>
+      <c r="D184">
+        <f t="shared" si="0"/>
+        <v>1.5441651030079551</v>
+      </c>
+      <c r="E184">
+        <v>202</v>
+      </c>
+      <c r="F184" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>45187</v>
+      </c>
+      <c r="B185">
+        <v>2242.58956979501</v>
+      </c>
+      <c r="C185">
+        <v>2215.13</v>
+      </c>
+      <c r="D185">
+        <f t="shared" si="0"/>
+        <v>1.2396369420760804</v>
+      </c>
+      <c r="E185">
+        <v>202</v>
+      </c>
+      <c r="F185" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>45187</v>
+      </c>
+      <c r="B186">
+        <v>2244.41489372865</v>
+      </c>
+      <c r="C186">
+        <v>2215.13</v>
+      </c>
+      <c r="D186">
+        <f t="shared" si="0"/>
+        <v>1.3220395068754374</v>
+      </c>
+      <c r="E186">
+        <v>202</v>
+      </c>
+      <c r="F186" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>45187</v>
+      </c>
+      <c r="B187">
+        <v>2243.4932476377799</v>
+      </c>
+      <c r="C187">
+        <v>2215.13</v>
+      </c>
+      <c r="D187">
+        <f t="shared" si="0"/>
+        <v>1.2804326444849625</v>
+      </c>
+      <c r="E187">
+        <v>202</v>
+      </c>
+      <c r="F187" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>45188</v>
+      </c>
+      <c r="B188">
+        <v>2225.1206910453502</v>
+      </c>
+      <c r="C188">
+        <v>2215.13</v>
+      </c>
+      <c r="D188">
+        <f t="shared" si="0"/>
+        <v>0.45102052905924728</v>
+      </c>
+      <c r="E188">
+        <v>202</v>
+      </c>
+      <c r="F188" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>45189</v>
+      </c>
+      <c r="B189">
+        <v>2234.4028838028098</v>
+      </c>
+      <c r="C189">
+        <v>2215.13</v>
+      </c>
+      <c r="D189">
+        <f t="shared" si="0"/>
+        <v>0.87005655662691128</v>
+      </c>
+      <c r="E189">
+        <v>202</v>
+      </c>
+      <c r="F189" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B190">
+        <v>2239.1234711340198</v>
+      </c>
+      <c r="C190">
+        <v>2215.13</v>
+      </c>
+      <c r="D190">
+        <f t="shared" si="0"/>
+        <v>1.0831631161159718</v>
+      </c>
+      <c r="E190">
+        <v>202</v>
+      </c>
+      <c r="F190" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B191">
+        <v>2243.3524489430401</v>
+      </c>
+      <c r="C191">
+        <v>2215.13</v>
+      </c>
+      <c r="D191">
+        <f t="shared" si="0"/>
+        <v>1.2740764173226868</v>
+      </c>
+      <c r="E191">
+        <v>202</v>
+      </c>
+      <c r="F191" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>45190</v>
+      </c>
+      <c r="B192">
+        <v>2237.2102815005401</v>
+      </c>
+      <c r="C192">
+        <v>2215.13</v>
+      </c>
+      <c r="D192">
+        <f t="shared" si="0"/>
+        <v>0.99679393536902872</v>
+      </c>
+      <c r="E192">
+        <v>202</v>
+      </c>
+      <c r="F192" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>45191</v>
+      </c>
+      <c r="B193">
+        <v>2240.2400110233002</v>
+      </c>
+      <c r="C193">
+        <v>2215.13</v>
+      </c>
+      <c r="D193">
+        <f t="shared" si="0"/>
+        <v>1.1335682792116084</v>
+      </c>
+      <c r="E193">
+        <v>202</v>
+      </c>
+      <c r="F193" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>45191</v>
+      </c>
+      <c r="B194">
+        <v>2238.1339013997799</v>
+      </c>
+      <c r="C194">
+        <v>2215.13</v>
+      </c>
+      <c r="D194">
+        <f t="shared" si="0"/>
+        <v>1.0384899035171662</v>
+      </c>
+      <c r="E194">
+        <v>202</v>
+      </c>
+      <c r="F194" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>45191</v>
+      </c>
+      <c r="B195">
+        <v>2237.75394506879</v>
+      </c>
+      <c r="C195">
+        <v>2215.13</v>
+      </c>
+      <c r="D195">
+        <f t="shared" si="0"/>
+        <v>1.0213371255316801</v>
+      </c>
+      <c r="E195">
+        <v>202</v>
+      </c>
+      <c r="F195" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>45191</v>
+      </c>
+      <c r="B196">
+        <v>2240.0742563691301</v>
+      </c>
+      <c r="C196">
+        <v>2215.13</v>
+      </c>
+      <c r="D196">
+        <f t="shared" si="0"/>
+        <v>1.1260854382871441</v>
+      </c>
+      <c r="E196">
+        <v>202</v>
+      </c>
+      <c r="F196" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>45194</v>
+      </c>
+      <c r="B197">
+        <v>2228.8756520000002</v>
+      </c>
+      <c r="C197">
+        <v>2215.13</v>
+      </c>
+      <c r="D197">
+        <f t="shared" ref="D197:D209" si="1">100*(B197-C197)/C197</f>
+        <v>0.62053477673996849</v>
+      </c>
+      <c r="E197">
+        <v>202</v>
+      </c>
+      <c r="F197" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>45195</v>
+      </c>
+      <c r="B198">
+        <v>2243.2235060349999</v>
+      </c>
+      <c r="C198">
+        <v>2215.13</v>
+      </c>
+      <c r="D198">
+        <f t="shared" si="1"/>
+        <v>1.2682554087118945</v>
+      </c>
+      <c r="E198">
+        <v>202</v>
+      </c>
+      <c r="F198" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>45195</v>
+      </c>
+      <c r="B199">
+        <v>2239.6614043404802</v>
+      </c>
+      <c r="C199">
+        <v>2215.13</v>
+      </c>
+      <c r="D199">
+        <f t="shared" si="1"/>
+        <v>1.1074476143829073</v>
+      </c>
+      <c r="E199">
+        <v>202</v>
+      </c>
+      <c r="F199" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>45198</v>
+      </c>
+      <c r="B200">
+        <v>2224.9684503119902</v>
+      </c>
+      <c r="C200">
+        <v>2215.13</v>
+      </c>
+      <c r="D200">
+        <f t="shared" si="1"/>
+        <v>0.44414776162076591</v>
+      </c>
+      <c r="E200">
+        <v>202</v>
+      </c>
+      <c r="F200" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>45201</v>
+      </c>
+      <c r="B201">
+        <v>2235.3029861474001</v>
+      </c>
+      <c r="C201">
+        <v>2215.13</v>
+      </c>
+      <c r="D201">
+        <f t="shared" si="1"/>
+        <v>0.91069084646950849</v>
+      </c>
+      <c r="E201">
+        <v>202</v>
+      </c>
+      <c r="F201" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>45202</v>
+      </c>
+      <c r="B202">
+        <v>2251.284661405</v>
+      </c>
+      <c r="C202">
+        <v>2230.52</v>
+      </c>
+      <c r="D202">
+        <f t="shared" si="1"/>
+        <v>0.93093365694994756</v>
+      </c>
+      <c r="E202">
+        <v>183</v>
+      </c>
+      <c r="F202" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>45202</v>
+      </c>
+      <c r="B203">
+        <v>2238.0063129999999</v>
+      </c>
+      <c r="C203">
+        <v>2220.62</v>
+      </c>
+      <c r="D203">
+        <f t="shared" si="1"/>
+        <v>0.78294859093406233</v>
+      </c>
+      <c r="E203">
+        <v>210</v>
+      </c>
+      <c r="F203" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>45202</v>
+      </c>
+      <c r="B204">
+        <v>2241.0215125582999</v>
+      </c>
+      <c r="C204">
+        <v>2220.62</v>
+      </c>
+      <c r="D204">
+        <f t="shared" si="1"/>
+        <v>0.91873046979222273</v>
+      </c>
+      <c r="E204">
+        <v>210</v>
+      </c>
+      <c r="F204" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>45203</v>
+      </c>
+      <c r="B205">
+        <v>2231.1387110542501</v>
+      </c>
+      <c r="C205">
+        <v>2220.62</v>
+      </c>
+      <c r="D205">
+        <f t="shared" si="1"/>
+        <v>0.47368352326152885</v>
+      </c>
+      <c r="E205">
+        <v>210</v>
+      </c>
+      <c r="F205" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>45203</v>
+      </c>
+      <c r="B206">
+        <v>2236.0169489530799</v>
+      </c>
+      <c r="C206">
+        <v>2220.62</v>
+      </c>
+      <c r="D206">
+        <f t="shared" si="1"/>
+        <v>0.69336261733570026</v>
+      </c>
+      <c r="E206">
+        <v>210</v>
+      </c>
+      <c r="F206" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>45204</v>
+      </c>
+      <c r="B207">
+        <v>2228.5572676656602</v>
+      </c>
+      <c r="C207">
+        <v>2220.62</v>
+      </c>
+      <c r="D207">
+        <f t="shared" si="1"/>
+        <v>0.35743475541336783</v>
+      </c>
+      <c r="E207">
+        <v>210</v>
+      </c>
+      <c r="F207" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>45205</v>
+      </c>
+      <c r="B208">
+        <v>2230.9677579999998</v>
+      </c>
+      <c r="C208">
+        <v>2220.62</v>
+      </c>
+      <c r="D208">
+        <f t="shared" si="1"/>
+        <v>0.46598508524645754</v>
+      </c>
+      <c r="E208">
+        <v>210</v>
+      </c>
+      <c r="F208" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>45246</v>
+      </c>
+      <c r="B209">
+        <v>2234.5253460253698</v>
+      </c>
+      <c r="C209">
+        <v>2220.62</v>
+      </c>
+      <c r="D209">
+        <f t="shared" si="1"/>
+        <v>0.62619205561374347</v>
+      </c>
+      <c r="E209">
+        <v>210</v>
+      </c>
+      <c r="F209" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>45251</v>
+      </c>
+      <c r="B210">
+        <v>2284.3929625445498</v>
+      </c>
+      <c r="C210">
+        <v>2220.62</v>
+      </c>
+      <c r="D210">
+        <f t="shared" ref="D210:D233" si="2">100*(B210-C210)/C210</f>
+        <v>2.8718539211819203</v>
+      </c>
+      <c r="E210">
+        <v>210</v>
+      </c>
+      <c r="F210" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>45251</v>
+      </c>
+      <c r="B211">
+        <v>2219</v>
+      </c>
+      <c r="C211">
+        <v>2220.62</v>
+      </c>
+      <c r="D211">
+        <f t="shared" si="2"/>
+        <v>-7.2952598823747009E-2</v>
+      </c>
+      <c r="E211">
+        <v>210</v>
+      </c>
+      <c r="F211" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>45252</v>
+      </c>
+      <c r="B212">
+        <v>2215.3307702611701</v>
+      </c>
+      <c r="C212">
+        <v>2220.62</v>
+      </c>
+      <c r="D212">
+        <f t="shared" si="2"/>
+        <v>-0.23818707112562337</v>
+      </c>
+      <c r="E212">
+        <v>210</v>
+      </c>
+      <c r="F212" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B213">
+        <v>2207.8233927312999</v>
+      </c>
+      <c r="C213">
+        <v>2220.62</v>
+      </c>
+      <c r="D213">
+        <f t="shared" si="2"/>
+        <v>-0.57626281257936851</v>
+      </c>
+      <c r="E213">
+        <v>210</v>
+      </c>
+      <c r="F213" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B214">
+        <v>2227.2938977260501</v>
+      </c>
+      <c r="C214">
+        <v>2220.62</v>
+      </c>
+      <c r="D214">
+        <f t="shared" si="2"/>
+        <v>0.30054208851808056</v>
+      </c>
+      <c r="E214">
+        <v>210</v>
+      </c>
+      <c r="F214" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B215">
+        <v>2218.0219911079298</v>
+      </c>
+      <c r="C215">
+        <v>2220.62</v>
+      </c>
+      <c r="D215">
+        <f t="shared" si="2"/>
+        <v>-0.11699475336032657</v>
+      </c>
+      <c r="E215">
+        <v>210</v>
+      </c>
+      <c r="F215" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B216">
+        <v>2217.40264475193</v>
+      </c>
+      <c r="C216">
+        <v>2220.62</v>
+      </c>
+      <c r="D216">
+        <f t="shared" si="2"/>
+        <v>-0.14488544857156593</v>
+      </c>
+      <c r="E216">
+        <v>210</v>
+      </c>
+      <c r="F216" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>45264</v>
+      </c>
+      <c r="B217">
+        <v>2241.7122277785502</v>
+      </c>
+      <c r="C217">
+        <v>2220.62</v>
+      </c>
+      <c r="D217">
+        <f t="shared" si="2"/>
+        <v>0.94983508112825688</v>
+      </c>
+      <c r="E217">
+        <v>210</v>
+      </c>
+      <c r="F217" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C218">
+        <v>2220.62</v>
+      </c>
+      <c r="D218">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+      <c r="F218" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>45265</v>
+      </c>
+      <c r="B219">
+        <v>2223.2911691568102</v>
+      </c>
+      <c r="C219">
+        <v>2220.62</v>
+      </c>
+      <c r="D219">
+        <f t="shared" si="2"/>
+        <v>0.12028934067108579</v>
+      </c>
+      <c r="E219">
+        <v>210</v>
+      </c>
+      <c r="F219" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>45266</v>
+      </c>
+      <c r="B220">
+        <v>2218.5324470355999</v>
+      </c>
+      <c r="C220">
+        <v>2220.62</v>
+      </c>
+      <c r="D220">
+        <f t="shared" si="2"/>
+        <v>-9.4007662922965085E-2</v>
+      </c>
+      <c r="E220">
+        <v>210</v>
+      </c>
+      <c r="F220" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>45266</v>
+      </c>
+      <c r="B221">
+        <v>2227.1876291475501</v>
+      </c>
+      <c r="C221">
+        <v>2220.62</v>
+      </c>
+      <c r="D221">
+        <f t="shared" si="2"/>
+        <v>0.29575655211383212</v>
+      </c>
+      <c r="E221">
+        <v>210</v>
+      </c>
+      <c r="F221" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>45267</v>
+      </c>
+      <c r="B222">
+        <v>2228.2490233854301</v>
+      </c>
+      <c r="C222">
+        <v>2220.62</v>
+      </c>
+      <c r="D222">
+        <f t="shared" si="2"/>
+        <v>0.34355375460142545</v>
+      </c>
+      <c r="E222">
+        <v>210</v>
+      </c>
+      <c r="F222" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>45275</v>
+      </c>
+      <c r="B223">
+        <v>2221.3274200628598</v>
+      </c>
+      <c r="C223">
+        <v>2220.62</v>
+      </c>
+      <c r="D223">
+        <f t="shared" si="2"/>
+        <v>3.1856871633143449E-2</v>
+      </c>
+      <c r="E223">
+        <v>210</v>
+      </c>
+      <c r="F223" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>45295</v>
+      </c>
+      <c r="B224">
+        <v>2198.79015104888</v>
+      </c>
+      <c r="C224">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D224">
+        <f t="shared" si="2"/>
+        <v>-0.37334557985710048</v>
+      </c>
+      <c r="E224">
+        <v>169</v>
+      </c>
+      <c r="F224" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>45296</v>
+      </c>
+      <c r="B225">
+        <v>2198.913689647</v>
+      </c>
+      <c r="C225">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D225">
+        <f t="shared" si="2"/>
+        <v>-0.3677480756038769</v>
+      </c>
+      <c r="E225">
+        <v>169</v>
+      </c>
+      <c r="F225" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>45299</v>
+      </c>
+      <c r="B226">
+        <v>2200.4298767319301</v>
+      </c>
+      <c r="C226">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D226">
+        <f t="shared" si="2"/>
+        <v>-0.29905000240459312</v>
+      </c>
+      <c r="E226">
+        <v>169</v>
+      </c>
+      <c r="F226" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>45300</v>
+      </c>
+      <c r="B227">
+        <v>2227.7367095242298</v>
+      </c>
+      <c r="C227">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D227">
+        <f t="shared" si="2"/>
+        <v>0.9382160425653302</v>
+      </c>
+      <c r="E227">
+        <v>169</v>
+      </c>
+      <c r="F227" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>45300</v>
+      </c>
+      <c r="B228">
+        <v>2221.9763666642598</v>
+      </c>
+      <c r="C228">
+        <v>2207.0300000000002</v>
+      </c>
+      <c r="D228">
+        <f t="shared" si="2"/>
+        <v>0.67721628905178377</v>
+      </c>
+      <c r="E228">
+        <v>169</v>
+      </c>
+      <c r="F228" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>45350</v>
+      </c>
+      <c r="B229">
+        <v>2205.93714193919</v>
+      </c>
+      <c r="C229" s="3">
+        <v>2193.54</v>
+      </c>
+      <c r="D229">
+        <f t="shared" si="2"/>
+        <v>0.56516598462713596</v>
+      </c>
+      <c r="E229">
+        <v>212</v>
+      </c>
+      <c r="F229" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>45351</v>
+      </c>
+      <c r="B230">
+        <v>2200.344286</v>
+      </c>
+      <c r="C230" s="3">
+        <v>2193.54</v>
+      </c>
+      <c r="D230">
+        <f t="shared" si="2"/>
+        <v>0.31019657722220917</v>
+      </c>
+      <c r="E230">
+        <v>212</v>
+      </c>
+      <c r="F230" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>45352</v>
+      </c>
+      <c r="B231">
+        <v>2207.8258852645099</v>
+      </c>
+      <c r="C231" s="3">
+        <v>2193.54</v>
+      </c>
+      <c r="D231">
+        <f t="shared" si="2"/>
+        <v>0.65127078897626411</v>
+      </c>
+      <c r="E231">
+        <v>212</v>
+      </c>
+      <c r="F231" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B232">
+        <v>2201.07013531344</v>
+      </c>
+      <c r="C232" s="3">
+        <v>2193.54</v>
+      </c>
+      <c r="D232">
+        <f t="shared" si="2"/>
+        <v>0.34328689303318116</v>
+      </c>
+      <c r="E232">
+        <v>212</v>
+      </c>
+      <c r="F232" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B233">
+        <v>2207.4374563487399</v>
+      </c>
+      <c r="C233" s="3">
+        <v>2193.54</v>
+      </c>
+      <c r="D233">
+        <f t="shared" si="2"/>
+        <v>0.63356293246259376</v>
+      </c>
+      <c r="E233">
+        <v>212</v>
+      </c>
+      <c r="F233" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>45381</v>
+      </c>
+      <c r="B234">
+        <v>2167</v>
+      </c>
+      <c r="C234" s="3">
+        <v>2193.54</v>
+      </c>
+      <c r="D234">
+        <f t="shared" ref="D234" si="3">100*(B234-C234)/C234</f>
+        <v>-1.2099163908567869</v>
+      </c>
+      <c r="E234">
+        <v>212</v>
+      </c>
+      <c r="F234" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rocky intertidal titrations 20240525
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -280,6 +280,15 @@
   </si>
   <si>
     <t>CRM opened 3/31/2024</t>
+  </si>
+  <si>
+    <t>CRM opened 5/21/2024</t>
+  </si>
+  <si>
+    <t>CRM opened 05/21/2024</t>
+  </si>
+  <si>
+    <t>CRM opened 5/21 , opened new batch of acid</t>
   </si>
 </sst>
 </file>
@@ -1101,11 +1110,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G238"/>
+  <dimension ref="A1:G246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F239" sqref="F239"/>
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E251" sqref="E251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5837,7 +5846,7 @@
         <v>2193.54</v>
       </c>
       <c r="D234">
-        <f t="shared" ref="D234:D238" si="3">100*(B234-C234)/C234</f>
+        <f t="shared" ref="D234:D246" si="3">100*(B234-C234)/C234</f>
         <v>-1.2099163908567869</v>
       </c>
       <c r="E234">
@@ -5929,6 +5938,173 @@
       </c>
       <c r="F238" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>45404</v>
+      </c>
+      <c r="B239">
+        <v>2231.97814827924</v>
+      </c>
+      <c r="C239" s="3">
+        <v>2230.52</v>
+      </c>
+      <c r="D239">
+        <f t="shared" si="3"/>
+        <v>6.5372571384253411E-2</v>
+      </c>
+      <c r="E239">
+        <v>183</v>
+      </c>
+      <c r="F239" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>45434</v>
+      </c>
+      <c r="B240">
+        <v>2228.69896965114</v>
+      </c>
+      <c r="C240" s="3">
+        <v>2215.13</v>
+      </c>
+      <c r="D240">
+        <f t="shared" si="3"/>
+        <v>0.6125586151214566</v>
+      </c>
+      <c r="E240">
+        <v>202</v>
+      </c>
+      <c r="F240" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>45433</v>
+      </c>
+      <c r="B241">
+        <v>2216.9235939999999</v>
+      </c>
+      <c r="C241">
+        <v>2215.13</v>
+      </c>
+      <c r="D241">
+        <v>8.0970159E-2</v>
+      </c>
+      <c r="E241">
+        <v>202</v>
+      </c>
+      <c r="F241" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>45435</v>
+      </c>
+      <c r="B242">
+        <v>2210.7065153475</v>
+      </c>
+      <c r="C242">
+        <v>2215.13</v>
+      </c>
+      <c r="D242">
+        <f t="shared" si="3"/>
+        <v>-0.19969413318857424</v>
+      </c>
+      <c r="E242">
+        <v>202</v>
+      </c>
+      <c r="F242" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>45437</v>
+      </c>
+      <c r="B243">
+        <v>2244.7447187303901</v>
+      </c>
+      <c r="C243">
+        <v>2215.13</v>
+      </c>
+      <c r="D243">
+        <f t="shared" si="3"/>
+        <v>1.3369291522569779</v>
+      </c>
+      <c r="E243">
+        <v>202</v>
+      </c>
+      <c r="F243" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>45437</v>
+      </c>
+      <c r="B244">
+        <v>2232.7867714721801</v>
+      </c>
+      <c r="C244">
+        <v>2215.13</v>
+      </c>
+      <c r="D244">
+        <f t="shared" si="3"/>
+        <v>0.79709865661067414</v>
+      </c>
+      <c r="E244">
+        <v>202</v>
+      </c>
+      <c r="F244" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>45437</v>
+      </c>
+      <c r="B245">
+        <v>2223.0452739453399</v>
+      </c>
+      <c r="C245">
+        <v>2215.13</v>
+      </c>
+      <c r="D245">
+        <f t="shared" si="3"/>
+        <v>0.35732773901937026</v>
+      </c>
+      <c r="E245">
+        <v>202</v>
+      </c>
+      <c r="F245" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>45437</v>
+      </c>
+      <c r="B246">
+        <v>2228.5157841463201</v>
+      </c>
+      <c r="C246">
+        <v>2215.13</v>
+      </c>
+      <c r="D246">
+        <f t="shared" si="3"/>
+        <v>0.60428887452745528</v>
+      </c>
+      <c r="E246">
+        <v>202</v>
+      </c>
+      <c r="F246" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sandy beach 2025_02_16 samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\labX_data\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CB9799-49C4-432D-A660-77579A401FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="7215" yWindow="2265" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -310,12 +324,15 @@
   </si>
   <si>
     <t>CRM opened 12/21/2024</t>
+  </si>
+  <si>
+    <t>CRM opened 02/19/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -805,12 +822,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1131,12 +1147,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G282"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D283" sqref="D283"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F284" sqref="F284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6644,7 +6660,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D271">
-        <f t="shared" ref="D271:D282" si="5">100*(B271-C271)/C271</f>
+        <f t="shared" ref="D271:D283" si="5">100*(B271-C271)/C271</f>
         <v>1.8486916817965684</v>
       </c>
       <c r="E271">
@@ -6679,20 +6695,20 @@
       <c r="A273" s="1">
         <v>45643</v>
       </c>
-      <c r="B273" s="4">
+      <c r="B273">
         <v>2229.1458608773301</v>
       </c>
-      <c r="C273" s="4">
+      <c r="C273">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D273" s="4">
+      <c r="D273">
         <f t="shared" si="5"/>
         <v>0.21020112104592337</v>
       </c>
-      <c r="E273" s="4">
+      <c r="E273">
         <v>217</v>
       </c>
-      <c r="F273" s="4" t="s">
+      <c r="F273" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6700,20 +6716,20 @@
       <c r="A274" s="1">
         <v>45643</v>
       </c>
-      <c r="B274" s="4">
+      <c r="B274">
         <v>2227.8164915082898</v>
       </c>
-      <c r="C274" s="4">
+      <c r="C274">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D274" s="4">
+      <c r="D274">
         <f t="shared" si="5"/>
         <v>0.1504399478657838</v>
       </c>
-      <c r="E274" s="4">
+      <c r="E274">
         <v>217</v>
       </c>
-      <c r="F274" s="4" t="s">
+      <c r="F274" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6721,20 +6737,20 @@
       <c r="A275" s="1">
         <v>45644</v>
       </c>
-      <c r="B275" s="4">
+      <c r="B275">
         <v>2227.8520852788101</v>
       </c>
-      <c r="C275" s="4">
+      <c r="C275">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D275" s="4">
+      <c r="D275">
         <f t="shared" si="5"/>
         <v>0.15204004903686438</v>
       </c>
-      <c r="E275" s="4">
+      <c r="E275">
         <v>217</v>
       </c>
-      <c r="F275" s="4" t="s">
+      <c r="F275" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6742,20 +6758,20 @@
       <c r="A276" s="1">
         <v>45644</v>
       </c>
-      <c r="B276" s="4">
+      <c r="B276">
         <v>2226.6731174644601</v>
       </c>
-      <c r="C276" s="4">
+      <c r="C276">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D276" s="4">
+      <c r="D276">
         <f t="shared" si="5"/>
         <v>9.9040106832653171E-2</v>
       </c>
-      <c r="E276" s="4">
+      <c r="E276">
         <v>217</v>
       </c>
-      <c r="F276" s="4" t="s">
+      <c r="F276" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6763,20 +6779,20 @@
       <c r="A277" s="1">
         <v>45645</v>
       </c>
-      <c r="B277" s="4">
+      <c r="B277">
         <v>2229.70694697415</v>
       </c>
-      <c r="C277" s="4">
+      <c r="C277">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D277" s="4">
+      <c r="D277">
         <f t="shared" si="5"/>
         <v>0.23542448197324373</v>
       </c>
       <c r="E277">
         <v>217</v>
       </c>
-      <c r="F277" s="4" t="s">
+      <c r="F277" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6784,20 +6800,20 @@
       <c r="A278" s="1">
         <v>45646</v>
       </c>
-      <c r="B278" s="4">
+      <c r="B278">
         <v>2232.6153441317001</v>
       </c>
-      <c r="C278" s="4">
+      <c r="C278">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D278" s="4">
+      <c r="D278">
         <f t="shared" si="5"/>
         <v>0.36617010486544271</v>
       </c>
-      <c r="E278" s="4">
+      <c r="E278">
         <v>217</v>
       </c>
-      <c r="F278" s="4" t="s">
+      <c r="F278" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6805,20 +6821,20 @@
       <c r="A279" s="1">
         <v>45646</v>
       </c>
-      <c r="B279" s="4">
+      <c r="B279">
         <v>2234.7378930379</v>
       </c>
-      <c r="C279" s="4">
+      <c r="C279">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D279" s="4">
+      <c r="D279">
         <f t="shared" si="5"/>
         <v>0.46158829015002201</v>
       </c>
       <c r="E279">
         <v>217</v>
       </c>
-      <c r="F279" s="4" t="s">
+      <c r="F279" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6826,17 +6842,17 @@
       <c r="A280" s="1">
         <v>45647</v>
       </c>
-      <c r="B280" s="4">
+      <c r="B280">
         <v>2230.18801681576</v>
       </c>
-      <c r="C280" s="4">
+      <c r="C280">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D280" s="4">
+      <c r="D280">
         <f t="shared" si="5"/>
         <v>0.2570507498757082</v>
       </c>
-      <c r="E280" s="4">
+      <c r="E280">
         <v>217</v>
       </c>
       <c r="F280" t="s">
@@ -6847,20 +6863,20 @@
       <c r="A281" s="1">
         <v>45647</v>
       </c>
-      <c r="B281" s="4">
+      <c r="B281">
         <v>2216.32655621186</v>
       </c>
-      <c r="C281" s="4">
+      <c r="C281">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D281" s="4">
+      <c r="D281">
         <f t="shared" si="5"/>
         <v>-0.36608467581670462</v>
       </c>
-      <c r="E281" s="4">
+      <c r="E281">
         <v>217</v>
       </c>
-      <c r="F281" s="4" t="s">
+      <c r="F281" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6868,21 +6884,42 @@
       <c r="A282" s="1">
         <v>45648</v>
       </c>
-      <c r="B282" s="4">
+      <c r="B282">
         <v>2240.49766278385</v>
       </c>
-      <c r="C282" s="4">
+      <c r="C282">
         <v>2224.4699999999998</v>
       </c>
-      <c r="D282" s="4">
+      <c r="D282">
         <f t="shared" si="5"/>
         <v>0.72051602331567732</v>
       </c>
       <c r="E282">
         <v>217</v>
       </c>
-      <c r="F282" s="4" t="s">
+      <c r="F282" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>45707</v>
+      </c>
+      <c r="B283">
+        <v>2200</v>
+      </c>
+      <c r="C283">
+        <v>2212.31</v>
+      </c>
+      <c r="D283">
+        <f t="shared" si="5"/>
+        <v>-0.55643196477889378</v>
+      </c>
+      <c r="E283">
+        <v>217</v>
+      </c>
+      <c r="F283" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sandy beach night 2025-03-11
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7F3262-D020-4178-A4BC-77EE4DD96DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02350C61-1B52-40FB-BC72-D9F816E518EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15705" yWindow="2415" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -1154,11 +1154,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G287"/>
+  <dimension ref="A1:G288"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F288" sqref="F288"/>
+      <selection pane="bottomLeft" activeCell="F292" sqref="F292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7002,13 +7002,34 @@
         <v>2213.31</v>
       </c>
       <c r="D287">
-        <f t="shared" ref="D287" si="8">100*(B287-C287)/C287</f>
+        <f t="shared" ref="D287:D288" si="8">100*(B287-C287)/C287</f>
         <v>-0.59474949284103729</v>
       </c>
       <c r="E287">
         <v>217</v>
       </c>
       <c r="F287" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>45730</v>
+      </c>
+      <c r="B288">
+        <v>2201.6959400000001</v>
+      </c>
+      <c r="C288">
+        <v>2213.31</v>
+      </c>
+      <c r="D288">
+        <f t="shared" si="8"/>
+        <v>-0.5247371583736522</v>
+      </c>
+      <c r="E288">
+        <v>217</v>
+      </c>
+      <c r="F288" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
diamond head night 2025-03-28
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB558B-85B8-45BA-8A7D-70B100BEB08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759CB14B-EA7E-4865-AB04-92C7D276B1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15705" yWindow="2415" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15315" yWindow="1185" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -1154,11 +1154,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G289"/>
+  <dimension ref="A1:G290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D294" sqref="D294"/>
+      <selection pane="bottomLeft" activeCell="C291" sqref="C291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7054,6 +7054,27 @@
         <v>97</v>
       </c>
     </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>45744</v>
+      </c>
+      <c r="B290">
+        <v>2203.6069900000002</v>
+      </c>
+      <c r="C290">
+        <v>2213.31</v>
+      </c>
+      <c r="D290">
+        <f t="shared" ref="D290" si="9">100*(B290-C290)/C290</f>
+        <v>-0.43839362764365236</v>
+      </c>
+      <c r="E290">
+        <v>217</v>
+      </c>
+      <c r="F290" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
made new folder and ran kaihalulu 2025-06-08
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286CA3B0-F003-4758-8B66-613EA87161E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C913A0-DBF5-43FF-B1CD-7F39DD3E11DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13110" yWindow="1125" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12810" yWindow="765" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>CRM opened on 04/14/2025</t>
+  </si>
+  <si>
+    <t>CRM opened on 06/10/2025</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1169,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G291"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
@@ -7108,6 +7111,27 @@
         <v>98</v>
       </c>
     </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>45818</v>
+      </c>
+      <c r="B292" s="4">
+        <v>2193.6378800000002</v>
+      </c>
+      <c r="C292">
+        <v>2212.31</v>
+      </c>
+      <c r="D292">
+        <f>100*(B292-C292)/C292</f>
+        <v>-0.84401010708262958</v>
+      </c>
+      <c r="E292">
+        <v>217</v>
+      </c>
+      <c r="F292" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran the rest of kaihalulu 2025-06-08
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C913A0-DBF5-43FF-B1CD-7F39DD3E11DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C34E07-11F4-4785-AC74-87F14AA1CFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12810" yWindow="765" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15255" yWindow="735" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -1169,11 +1169,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G292"/>
+  <dimension ref="A1:G293"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E293" sqref="E293"/>
+      <selection pane="bottomLeft" activeCell="E293" sqref="E293:F293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7132,6 +7132,27 @@
         <v>99</v>
       </c>
     </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>45820</v>
+      </c>
+      <c r="B293" s="4">
+        <v>2195.2128299999999</v>
+      </c>
+      <c r="C293">
+        <v>2212.31</v>
+      </c>
+      <c r="D293">
+        <f>100*(B293-C293)/C293</f>
+        <v>-0.77281981277488265</v>
+      </c>
+      <c r="E293">
+        <v>217</v>
+      </c>
+      <c r="F293" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ran CRM, practicing GitHub
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9655E3BF-418A-47EC-8B4F-E286A7F8B577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8001BB-B8E6-4026-9AF5-BDACCC68DF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15255" yWindow="735" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -1169,11 +1169,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G294"/>
+  <dimension ref="A1:G295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F298" sqref="F298"/>
+      <selection pane="bottomLeft" activeCell="A296" sqref="A296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7174,6 +7174,27 @@
         <v>99</v>
       </c>
     </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>45833</v>
+      </c>
+      <c r="B295" s="4">
+        <v>2191.2403300000001</v>
+      </c>
+      <c r="C295">
+        <v>2212.31</v>
+      </c>
+      <c r="D295">
+        <f>100*(B295-C295)/C295</f>
+        <v>-0.9523832555112014</v>
+      </c>
+      <c r="E295">
+        <v>217</v>
+      </c>
+      <c r="F295" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran kaihalulu 2025-07-20 all samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8001BB-B8E6-4026-9AF5-BDACCC68DF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116E9B81-27BD-4255-854B-D75636AF2BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15255" yWindow="735" windowWidth="13005" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15675" yWindow="300" windowWidth="13080" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>CRM opened on 06/10/2025</t>
+  </si>
+  <si>
+    <t>CRM opened on 06/10/2025, will replace</t>
+  </si>
+  <si>
+    <t>CRM opened on 07/22/2025</t>
   </si>
 </sst>
 </file>
@@ -1169,11 +1175,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G295"/>
+  <dimension ref="A1:G297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A296" sqref="A296"/>
+      <selection pane="bottomLeft" activeCell="C297" sqref="C297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7195,6 +7201,48 @@
         <v>99</v>
       </c>
     </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>45860</v>
+      </c>
+      <c r="B296" s="4">
+        <v>2185.3806199999999</v>
+      </c>
+      <c r="C296">
+        <v>2212.31</v>
+      </c>
+      <c r="D296">
+        <f>100*(B296-C296)/C296</f>
+        <v>-1.2172516509892393</v>
+      </c>
+      <c r="E296">
+        <v>217</v>
+      </c>
+      <c r="F296" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>45860</v>
+      </c>
+      <c r="B297" s="4">
+        <v>2195.7069999999999</v>
+      </c>
+      <c r="C297">
+        <v>2212.31</v>
+      </c>
+      <c r="D297">
+        <f>100*(B297-C297)/C297</f>
+        <v>-0.75048252731308296</v>
+      </c>
+      <c r="E297">
+        <v>217</v>
+      </c>
+      <c r="F297" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran kaihalulu 2025-07-20 part 1
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116E9B81-27BD-4255-854B-D75636AF2BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410ED327-1766-4E12-B46C-02ADB2B0CC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15675" yWindow="300" windowWidth="13080" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -1175,11 +1175,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G297"/>
+  <dimension ref="A1:G298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C297" sqref="C297"/>
+      <selection pane="bottomLeft" activeCell="D300" sqref="D300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7107,7 +7107,7 @@
         <v>2212.31</v>
       </c>
       <c r="D291">
-        <f>100*(B291-C291)/C291</f>
+        <f t="shared" ref="D291:D298" si="10">100*(B291-C291)/C291</f>
         <v>-1.8699458936580336E-2</v>
       </c>
       <c r="E291">
@@ -7128,7 +7128,7 @@
         <v>2212.31</v>
       </c>
       <c r="D292">
-        <f>100*(B292-C292)/C292</f>
+        <f t="shared" si="10"/>
         <v>-0.84401010708262958</v>
       </c>
       <c r="E292">
@@ -7149,7 +7149,7 @@
         <v>2212.31</v>
       </c>
       <c r="D293">
-        <f>100*(B293-C293)/C293</f>
+        <f t="shared" si="10"/>
         <v>-0.77281981277488265</v>
       </c>
       <c r="E293">
@@ -7170,7 +7170,7 @@
         <v>2212.31</v>
       </c>
       <c r="D294">
-        <f>100*(B294-C294)/C294</f>
+        <f t="shared" si="10"/>
         <v>-0.61225641976033285</v>
       </c>
       <c r="E294">
@@ -7191,7 +7191,7 @@
         <v>2212.31</v>
       </c>
       <c r="D295">
-        <f>100*(B295-C295)/C295</f>
+        <f t="shared" si="10"/>
         <v>-0.9523832555112014</v>
       </c>
       <c r="E295">
@@ -7212,7 +7212,7 @@
         <v>2212.31</v>
       </c>
       <c r="D296">
-        <f>100*(B296-C296)/C296</f>
+        <f t="shared" si="10"/>
         <v>-1.2172516509892393</v>
       </c>
       <c r="E296">
@@ -7233,13 +7233,34 @@
         <v>2212.31</v>
       </c>
       <c r="D297">
-        <f>100*(B297-C297)/C297</f>
+        <f t="shared" si="10"/>
         <v>-0.75048252731308296</v>
       </c>
       <c r="E297">
         <v>217</v>
       </c>
       <c r="F297" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>45867</v>
+      </c>
+      <c r="B298" s="4">
+        <v>2193.57456</v>
+      </c>
+      <c r="C298">
+        <v>2212.31</v>
+      </c>
+      <c r="D298">
+        <f t="shared" si="10"/>
+        <v>-0.84687227377717977</v>
+      </c>
+      <c r="E298">
+        <v>217</v>
+      </c>
+      <c r="F298" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran kaihalulu 2025-07-26 part 2
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410ED327-1766-4E12-B46C-02ADB2B0CC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9019987A-48BC-4ED2-902E-F872727358A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15675" yWindow="300" windowWidth="13080" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -1175,11 +1175,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G298"/>
+  <dimension ref="A1:G299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D300" sqref="D300"/>
+      <selection pane="bottomLeft" activeCell="F300" sqref="F300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7107,7 +7107,7 @@
         <v>2212.31</v>
       </c>
       <c r="D291">
-        <f t="shared" ref="D291:D298" si="10">100*(B291-C291)/C291</f>
+        <f t="shared" ref="D291:D299" si="10">100*(B291-C291)/C291</f>
         <v>-1.8699458936580336E-2</v>
       </c>
       <c r="E291">
@@ -7261,6 +7261,27 @@
         <v>217</v>
       </c>
       <c r="F298" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>45868</v>
+      </c>
+      <c r="B299" s="4">
+        <v>2193.4159</v>
+      </c>
+      <c r="C299">
+        <v>2212.31</v>
+      </c>
+      <c r="D299">
+        <f t="shared" si="10"/>
+        <v>-0.85404396309739505</v>
+      </c>
+      <c r="E299">
+        <v>217</v>
+      </c>
+      <c r="F299" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tried to run sandy 2025-11-05
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9019987A-48BC-4ED2-902E-F872727358A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D79C87-4748-4446-8153-C07DD0227546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15675" yWindow="300" windowWidth="13080" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11685" yWindow="1650" windowWidth="13080" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="105">
   <si>
     <t>Date</t>
   </si>
@@ -339,6 +340,15 @@
   </si>
   <si>
     <t>CRM opened on 07/22/2025</t>
+  </si>
+  <si>
+    <t>CRM opened on 11/10/2025, will run again</t>
+  </si>
+  <si>
+    <t>same CRM ran again but noticed acid is low and may have had bubbles, will refill acid (same batch A28) and run crm again</t>
+  </si>
+  <si>
+    <t>same CRM, giving up, trying again a different day</t>
   </si>
 </sst>
 </file>
@@ -1175,11 +1185,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G299"/>
+  <dimension ref="A1:G302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F300" sqref="F300"/>
+      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F303" sqref="F303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7107,7 +7117,7 @@
         <v>2212.31</v>
       </c>
       <c r="D291">
-        <f t="shared" ref="D291:D299" si="10">100*(B291-C291)/C291</f>
+        <f t="shared" ref="D291:D302" si="10">100*(B291-C291)/C291</f>
         <v>-1.8699458936580336E-2</v>
       </c>
       <c r="E291">
@@ -7283,6 +7293,69 @@
       </c>
       <c r="F299" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>45971</v>
+      </c>
+      <c r="B300" s="4">
+        <v>2177.01359</v>
+      </c>
+      <c r="C300">
+        <v>2212.31</v>
+      </c>
+      <c r="D300">
+        <f t="shared" si="10"/>
+        <v>-1.5954549769245687</v>
+      </c>
+      <c r="E300">
+        <v>217</v>
+      </c>
+      <c r="F300" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>45971</v>
+      </c>
+      <c r="B301" s="4">
+        <v>2161.3153600000001</v>
+      </c>
+      <c r="C301">
+        <v>2212.31</v>
+      </c>
+      <c r="D301">
+        <f t="shared" si="10"/>
+        <v>-2.3050404328507259</v>
+      </c>
+      <c r="E301">
+        <v>217</v>
+      </c>
+      <c r="F301" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>45971</v>
+      </c>
+      <c r="B302" s="4">
+        <v>2182.5608900000002</v>
+      </c>
+      <c r="C302">
+        <v>2212.31</v>
+      </c>
+      <c r="D302">
+        <f t="shared" si="10"/>
+        <v>-1.3447080201237507</v>
+      </c>
+      <c r="E302">
+        <v>217</v>
+      </c>
+      <c r="F302" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran 1/2 sandy 2025-11-05
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D79C87-4748-4446-8153-C07DD0227546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A45DA6-242E-415A-8802-6C2F2511A959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11685" yWindow="1650" windowWidth="13080" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15525" yWindow="1065" windowWidth="12960" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -349,6 +348,9 @@
   </si>
   <si>
     <t>same CRM, giving up, trying again a different day</t>
+  </si>
+  <si>
+    <t>same CRM opened 11/10/2025, actually good this time</t>
   </si>
 </sst>
 </file>
@@ -1185,11 +1187,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G302"/>
+  <dimension ref="A1:G303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F303" sqref="F303"/>
+      <selection pane="bottomLeft" activeCell="F304" sqref="F304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7117,7 +7119,7 @@
         <v>2212.31</v>
       </c>
       <c r="D291">
-        <f t="shared" ref="D291:D302" si="10">100*(B291-C291)/C291</f>
+        <f t="shared" ref="D291:D303" si="10">100*(B291-C291)/C291</f>
         <v>-1.8699458936580336E-2</v>
       </c>
       <c r="E291">
@@ -7356,6 +7358,27 @@
       </c>
       <c r="F302" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>45974</v>
+      </c>
+      <c r="B303" s="4">
+        <v>2204.3165600000002</v>
+      </c>
+      <c r="C303">
+        <v>2212.31</v>
+      </c>
+      <c r="D303">
+        <f t="shared" si="10"/>
+        <v>-0.36131645203428708</v>
+      </c>
+      <c r="E303">
+        <v>217</v>
+      </c>
+      <c r="F303" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sandy 2025-11-05 part 2
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A45DA6-242E-415A-8802-6C2F2511A959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32528144-278F-4545-9B06-094CABB484CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15525" yWindow="1065" windowWidth="12960" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>same CRM opened 11/10/2025, actually good this time</t>
+  </si>
+  <si>
+    <t>same CRM, ran another one for second set of samples</t>
   </si>
 </sst>
 </file>
@@ -1187,11 +1190,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G303"/>
+  <dimension ref="A1:G304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F304" sqref="F304"/>
+      <selection pane="bottomLeft" activeCell="F305" sqref="F305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7119,7 +7122,7 @@
         <v>2212.31</v>
       </c>
       <c r="D291">
-        <f t="shared" ref="D291:D303" si="10">100*(B291-C291)/C291</f>
+        <f t="shared" ref="D291:D304" si="10">100*(B291-C291)/C291</f>
         <v>-1.8699458936580336E-2</v>
       </c>
       <c r="E291">
@@ -7379,6 +7382,27 @@
       </c>
       <c r="F303" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>45974</v>
+      </c>
+      <c r="B304" s="4">
+        <v>2203.0845800000002</v>
+      </c>
+      <c r="C304">
+        <v>2212.31</v>
+      </c>
+      <c r="D304">
+        <f t="shared" si="10"/>
+        <v>-0.41700394610157521</v>
+      </c>
+      <c r="E304">
+        <v>217</v>
+      </c>
+      <c r="F304" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mica summer samples re-run part 1
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32528144-278F-4545-9B06-094CABB484CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385B34AE-2CE9-42B3-B21A-D95090DCEDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15525" yWindow="1065" windowWidth="12960" windowHeight="11445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14715" yWindow="1065" windowWidth="13770" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>same CRM, ran another one for second set of samples</t>
+  </si>
+  <si>
+    <t>same CRM opened 11/10/2025</t>
+  </si>
+  <si>
+    <t>Testing an old CRM IGNORE</t>
   </si>
 </sst>
 </file>
@@ -1190,11 +1196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G304"/>
+  <dimension ref="A1:G306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F305" sqref="F305"/>
+      <selection pane="bottomLeft" activeCell="E313" sqref="E313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7122,7 +7128,7 @@
         <v>2212.31</v>
       </c>
       <c r="D291">
-        <f t="shared" ref="D291:D304" si="10">100*(B291-C291)/C291</f>
+        <f t="shared" ref="D291:D306" si="10">100*(B291-C291)/C291</f>
         <v>-1.8699458936580336E-2</v>
       </c>
       <c r="E291">
@@ -7403,6 +7409,48 @@
       </c>
       <c r="F304" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>45985</v>
+      </c>
+      <c r="B305" s="4">
+        <v>2196.3349600000001</v>
+      </c>
+      <c r="C305">
+        <v>2212.31</v>
+      </c>
+      <c r="D305">
+        <f t="shared" si="10"/>
+        <v>-0.72209771686607249</v>
+      </c>
+      <c r="E305">
+        <v>217</v>
+      </c>
+      <c r="F305" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>45985</v>
+      </c>
+      <c r="B306" s="4">
+        <v>2204.1925099999999</v>
+      </c>
+      <c r="C306">
+        <v>2212.31</v>
+      </c>
+      <c r="D306">
+        <f t="shared" si="10"/>
+        <v>-0.36692371322283446</v>
+      </c>
+      <c r="E306">
+        <v>217</v>
+      </c>
+      <c r="F306" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding test files mp
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385B34AE-2CE9-42B3-B21A-D95090DCEDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006F5782-D940-4395-8F25-9CD30DBC5659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14715" yWindow="1065" windowWidth="13770" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="570" windowWidth="12000" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>Testing an old CRM IGNORE</t>
+  </si>
+  <si>
+    <t>same CRM opened 11/10/2025, ignoring bc test, will retry and open new if bad next week</t>
   </si>
 </sst>
 </file>
@@ -1196,11 +1199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G306"/>
+  <dimension ref="A1:G307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E313" sqref="E313"/>
+      <selection pane="bottomLeft" activeCell="F308" sqref="F308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7128,7 +7131,7 @@
         <v>2212.31</v>
       </c>
       <c r="D291">
-        <f t="shared" ref="D291:D306" si="10">100*(B291-C291)/C291</f>
+        <f t="shared" ref="D291:D307" si="10">100*(B291-C291)/C291</f>
         <v>-1.8699458936580336E-2</v>
       </c>
       <c r="E291">
@@ -7451,6 +7454,27 @@
       </c>
       <c r="F306" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>46062</v>
+      </c>
+      <c r="B307" s="4">
+        <v>2262.82393</v>
+      </c>
+      <c r="C307">
+        <v>2212.31</v>
+      </c>
+      <c r="D307">
+        <f t="shared" si="10"/>
+        <v>2.2833115612188197</v>
+      </c>
+      <c r="E307">
+        <v>217</v>
+      </c>
+      <c r="F307" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran Sandy 2026-02-22 part 2
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911C222B-618E-41E1-82FD-0DA3532CA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A58CEEF-8FAD-41FC-92A5-EE8C1CECE8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15585" yWindow="720" windowWidth="13215" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>new CRM opened 02/23/2026</t>
+  </si>
+  <si>
+    <t>same CRM opened 02/23/2026</t>
   </si>
 </sst>
 </file>
@@ -1202,11 +1205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G308"/>
+  <dimension ref="A1:G309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C316" sqref="C316"/>
+      <selection pane="bottomLeft" activeCell="F313" sqref="F313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7501,6 +7504,27 @@
         <v>110</v>
       </c>
     </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
+        <v>46077</v>
+      </c>
+      <c r="B309" s="4">
+        <v>2202.3117900000002</v>
+      </c>
+      <c r="C309">
+        <v>2212.31</v>
+      </c>
+      <c r="D309">
+        <f t="shared" ref="D309" si="11">100*(B309-C309)/C309</f>
+        <v>-0.45193530743881938</v>
+      </c>
+      <c r="E309">
+        <v>217</v>
+      </c>
+      <c r="F309" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>